<commit_message>
5.2 changes in text
</commit_message>
<xml_diff>
--- a/Index_of_terms.xlsx
+++ b/Index_of_terms.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steffi\Documents\work\schmettow\GitHub\New_Stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C646FB0-7074-4225-8BBE-77C352875991}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DDDA79F-EB24-4DE2-9487-E19BDDB69C81}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="206">
   <si>
     <t>Term</t>
   </si>
@@ -607,6 +607,48 @@
   </si>
   <si>
     <t>an object in which multiple values of the same data type can be stored.</t>
+  </si>
+  <si>
+    <t>Smoother</t>
+  </si>
+  <si>
+    <t>A line indicating the average of values in a plot, e.g. LOESS (locally estimated scatterplot smoothing).</t>
+  </si>
+  <si>
+    <t>Covariate</t>
+  </si>
+  <si>
+    <t>Predictor</t>
+  </si>
+  <si>
+    <t>5.2.1</t>
+  </si>
+  <si>
+    <t>Centering of a predictor</t>
+  </si>
+  <si>
+    <t>Shifting of a predictor</t>
+  </si>
+  <si>
+    <t>Random walk</t>
+  </si>
+  <si>
+    <t>Standard deviation</t>
+  </si>
+  <si>
+    <t>Bootstrapping</t>
+  </si>
+  <si>
+    <t>Correlation</t>
+  </si>
+  <si>
+    <t>5.2.2</t>
+  </si>
+  <si>
+    <t>Covariance</t>
+  </si>
+  <si>
+    <t>Posterior</t>
   </si>
 </sst>
 </file>
@@ -937,10 +979,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1009,559 +1051,523 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D5" t="s">
-        <v>116</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>105</v>
-      </c>
-      <c r="B7" t="s">
-        <v>106</v>
+        <v>197</v>
       </c>
       <c r="C7" t="s">
-        <v>119</v>
-      </c>
-      <c r="D7" t="s">
-        <v>120</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="2">
-        <v>4</v>
+        <v>118</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>105</v>
       </c>
       <c r="B9" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>119</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>112</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>124</v>
-      </c>
-      <c r="C10" t="s">
-        <v>122</v>
+        <v>39</v>
+      </c>
+      <c r="C10" s="2">
+        <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>123</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>160</v>
+        <v>121</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
       <c r="B12" t="s">
-        <v>161</v>
+        <v>124</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>122</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>85</v>
-      </c>
-      <c r="B14" t="s">
-        <v>86</v>
+        <v>202</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14" t="s">
-        <v>125</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>93</v>
-      </c>
-      <c r="B15" t="s">
-        <v>94</v>
-      </c>
-      <c r="C15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" t="s">
-        <v>62</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" t="s">
-        <v>76</v>
+        <v>194</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" t="s">
-        <v>126</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>113</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C17" t="s">
-        <v>128</v>
+        <v>57</v>
       </c>
       <c r="D17" t="s">
-        <v>127</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>102</v>
-      </c>
-      <c r="C18" s="2">
-        <v>4</v>
+        <v>162</v>
+      </c>
+      <c r="C18" t="s">
+        <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="B19" t="s">
-        <v>103</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>129</v>
+        <v>86</v>
+      </c>
+      <c r="C19" t="s">
+        <v>64</v>
       </c>
       <c r="D19" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>93</v>
       </c>
       <c r="B20" t="s">
-        <v>164</v>
+        <v>94</v>
       </c>
       <c r="C20" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="C21" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="D21" t="s">
-        <v>62</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>82</v>
+        <v>113</v>
       </c>
       <c r="B22" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="D22" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>166</v>
-      </c>
-      <c r="C23" t="s">
-        <v>63</v>
+        <v>102</v>
+      </c>
+      <c r="C23" s="2">
+        <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>132</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B24" t="s">
-        <v>98</v>
-      </c>
-      <c r="C24" t="s">
-        <v>133</v>
+        <v>103</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="D24" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D25" t="s">
-        <v>57</v>
+        <v>46</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>110</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>168</v>
+        <v>16</v>
+      </c>
+      <c r="B26" t="s">
+        <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>135</v>
+        <v>63</v>
       </c>
       <c r="D26" t="s">
-        <v>136</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>169</v>
+        <v>82</v>
+      </c>
+      <c r="B27" t="s">
+        <v>165</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D27" t="s">
-        <v>65</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>95</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>188</v>
+        <v>17</v>
+      </c>
+      <c r="B28" t="s">
+        <v>166</v>
       </c>
       <c r="C28" t="s">
-        <v>133</v>
+        <v>63</v>
       </c>
       <c r="D28" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>20</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>170</v>
+        <v>97</v>
+      </c>
+      <c r="B29" t="s">
+        <v>98</v>
       </c>
       <c r="C29" t="s">
-        <v>49</v>
+        <v>133</v>
       </c>
       <c r="D29" t="s">
-        <v>66</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>167</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D30" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>68</v>
-      </c>
-      <c r="B31" t="s">
-        <v>171</v>
+        <v>110</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>168</v>
       </c>
       <c r="C31" t="s">
-        <v>46</v>
+        <v>135</v>
       </c>
       <c r="D31" t="s">
-        <v>69</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C32" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="D32" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>100</v>
-      </c>
-      <c r="B33" t="s">
-        <v>99</v>
+        <v>95</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="C33" t="s">
-        <v>59</v>
+        <v>133</v>
       </c>
       <c r="D33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>111</v>
-      </c>
-      <c r="B34" t="s">
-        <v>173</v>
+        <v>20</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>170</v>
       </c>
       <c r="C34" t="s">
-        <v>139</v>
+        <v>49</v>
       </c>
       <c r="D34" t="s">
-        <v>140</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="B35" t="s">
-        <v>174</v>
+        <v>41</v>
       </c>
       <c r="C35" t="s">
-        <v>141</v>
+        <v>55</v>
       </c>
       <c r="D35" t="s">
-        <v>142</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="B36" t="s">
-        <v>77</v>
+        <v>171</v>
       </c>
       <c r="C36" t="s">
         <v>46</v>
       </c>
       <c r="D36" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>88</v>
-      </c>
-      <c r="B37" t="s">
-        <v>175</v>
+        <v>22</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>172</v>
       </c>
       <c r="C37" t="s">
-        <v>115</v>
+        <v>70</v>
       </c>
       <c r="D37" t="s">
-        <v>132</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="B38" t="s">
-        <v>176</v>
+        <v>99</v>
       </c>
       <c r="C38" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="D38" t="s">
-        <v>73</v>
+        <v>138</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>25</v>
+        <v>111</v>
       </c>
       <c r="B39" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C39" t="s">
-        <v>46</v>
+        <v>139</v>
       </c>
       <c r="D39" t="s">
-        <v>62</v>
+        <v>140</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>26</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>178</v>
+        <v>84</v>
+      </c>
+      <c r="B40" t="s">
+        <v>174</v>
       </c>
       <c r="C40" t="s">
-        <v>49</v>
+        <v>141</v>
       </c>
       <c r="D40" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>89</v>
+        <v>23</v>
       </c>
       <c r="B41" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="C41" t="s">
-        <v>133</v>
+        <v>46</v>
       </c>
       <c r="D41" t="s">
-        <v>132</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
       <c r="B42" t="s">
-        <v>101</v>
+        <v>175</v>
       </c>
       <c r="C42" t="s">
-        <v>57</v>
+        <v>115</v>
       </c>
       <c r="D42" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B43" t="s">
-        <v>42</v>
+        <v>176</v>
       </c>
       <c r="C43" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D43" t="s">
-        <v>145</v>
+        <v>73</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="B44" t="s">
-        <v>81</v>
+        <v>177</v>
       </c>
       <c r="C44" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D44" t="s">
         <v>62</v>
@@ -1569,69 +1575,69 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>91</v>
-      </c>
-      <c r="B45" t="s">
-        <v>92</v>
+        <v>26</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>178</v>
       </c>
       <c r="C45" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D45" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="B46" t="s">
-        <v>179</v>
+        <v>90</v>
       </c>
       <c r="C46" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D46" t="s">
-        <v>62</v>
+        <v>132</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>83</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>180</v>
+        <v>27</v>
+      </c>
+      <c r="B47" t="s">
+        <v>101</v>
       </c>
       <c r="C47" t="s">
-        <v>147</v>
+        <v>57</v>
       </c>
       <c r="D47" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B48" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="C48" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D48" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="B49" t="s">
-        <v>43</v>
-      </c>
-      <c r="C49" s="2">
-        <v>4</v>
+        <v>81</v>
+      </c>
+      <c r="C49" t="s">
+        <v>49</v>
       </c>
       <c r="D49" t="s">
         <v>62</v>
@@ -1639,183 +1645,298 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="B50" t="s">
-        <v>181</v>
+        <v>92</v>
       </c>
       <c r="C50" t="s">
-        <v>149</v>
+        <v>46</v>
       </c>
       <c r="D50" t="s">
-        <v>62</v>
+        <v>146</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>108</v>
+        <v>29</v>
       </c>
       <c r="B51" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C51" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="D51" t="s">
-        <v>151</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>109</v>
-      </c>
-      <c r="B52" t="s">
-        <v>183</v>
+        <v>83</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>180</v>
       </c>
       <c r="C52" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D52" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B53" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="C53" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D53" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>184</v>
-      </c>
-      <c r="B54" t="s">
-        <v>185</v>
-      </c>
-      <c r="C54" t="s">
-        <v>153</v>
-      </c>
-      <c r="D54" t="s">
-        <v>154</v>
+        <v>205</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>33</v>
-      </c>
-      <c r="B55" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="C55" t="s">
-        <v>49</v>
-      </c>
-      <c r="D55" t="s">
-        <v>155</v>
+        <v>196</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B56" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="C56" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D56" t="s">
-        <v>138</v>
+        <v>62</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>35</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="C57" s="2">
-        <v>4</v>
-      </c>
-      <c r="D57" t="s">
-        <v>156</v>
+        <v>199</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>36</v>
+        <v>107</v>
       </c>
       <c r="B58" t="s">
-        <v>45</v>
-      </c>
-      <c r="C58" s="2">
-        <v>4</v>
+        <v>181</v>
+      </c>
+      <c r="C58" t="s">
+        <v>149</v>
       </c>
       <c r="D58" t="s">
-        <v>157</v>
+        <v>62</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>96</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>188</v>
+        <v>108</v>
+      </c>
+      <c r="B59" t="s">
+        <v>182</v>
       </c>
       <c r="C59" t="s">
-        <v>46</v>
+        <v>150</v>
       </c>
       <c r="D59" t="s">
-        <v>62</v>
+        <v>151</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>114</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>189</v>
+        <v>109</v>
+      </c>
+      <c r="B60" t="s">
+        <v>183</v>
       </c>
       <c r="C60" t="s">
-        <v>59</v>
+        <v>150</v>
       </c>
       <c r="D60" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B61" t="s">
-        <v>190</v>
+        <v>44</v>
       </c>
       <c r="C61" t="s">
-        <v>122</v>
+        <v>55</v>
       </c>
       <c r="D61" t="s">
-        <v>62</v>
+        <v>139</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
+        <v>184</v>
+      </c>
+      <c r="B62" t="s">
+        <v>185</v>
+      </c>
+      <c r="C62" t="s">
+        <v>153</v>
+      </c>
+      <c r="D62" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>33</v>
+      </c>
+      <c r="B63" t="s">
+        <v>186</v>
+      </c>
+      <c r="C63" t="s">
+        <v>49</v>
+      </c>
+      <c r="D63" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>198</v>
+      </c>
+      <c r="C64" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>192</v>
+      </c>
+      <c r="B65" t="s">
+        <v>193</v>
+      </c>
+      <c r="C65" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>34</v>
+      </c>
+      <c r="B67" t="s">
+        <v>79</v>
+      </c>
+      <c r="C67" s="2">
+        <v>1</v>
+      </c>
+      <c r="D67" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>35</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C68" s="2">
+        <v>4</v>
+      </c>
+      <c r="D68" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>36</v>
+      </c>
+      <c r="B69" t="s">
+        <v>45</v>
+      </c>
+      <c r="C69" s="2">
+        <v>4</v>
+      </c>
+      <c r="D69" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>96</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C70" t="s">
+        <v>46</v>
+      </c>
+      <c r="D70" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>114</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C71" t="s">
+        <v>59</v>
+      </c>
+      <c r="D71" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>37</v>
+      </c>
+      <c r="B72" t="s">
+        <v>190</v>
+      </c>
+      <c r="C72" t="s">
+        <v>122</v>
+      </c>
+      <c r="D72" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
         <v>38</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B73" t="s">
         <v>191</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C73" t="s">
         <v>64</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D73" t="s">
         <v>159</v>
       </c>
     </row>

</xml_diff>

<commit_message>
glossary, issues fixing, 6-6.2
</commit_message>
<xml_diff>
--- a/Index_of_terms.xlsx
+++ b/Index_of_terms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steffi\Documents\work\schmettow\GitHub\New_Stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0422DB8E-C0CE-42B6-ACE8-E60CD47F5FA9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A496FC-AC01-483B-B8E9-8E61346798B6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="407">
   <si>
     <t>Term</t>
   </si>
@@ -781,9 +781,6 @@
   </si>
   <si>
     <t>5.1.1</t>
-  </si>
-  <si>
-    <t>Quartile</t>
   </si>
   <si>
     <t>Inferential statistics</t>
@@ -1177,6 +1174,96 @@
   </si>
   <si>
     <t>a (non-defined) cause for residuals.</t>
+  </si>
+  <si>
+    <t>potentially relevant traits are recorded and equal composition of the groups is aspired.</t>
+  </si>
+  <si>
+    <t>also called bivariate correlation, symbol r. Used to calculate a linear correlation by deviding the covariance of x and y by the product of the two standard deviations.</t>
+  </si>
+  <si>
+    <t>All subjects or object one wants to make statements about.</t>
+  </si>
+  <si>
+    <t>The sample used in the study is representative for the population.</t>
+  </si>
+  <si>
+    <t>A variable used to estimate another variable, also called independent variable.</t>
+  </si>
+  <si>
+    <t>Certain characteristic variables are proportionally equal distributed across the sample as they are in the population.</t>
+  </si>
+  <si>
+    <t>a quantile splits the data into equal amounts of data points, e.g. the 50% quantile is the median.</t>
+  </si>
+  <si>
+    <t>a q-q plot compares the quantiles of each data point with quantiles from a normal distribution.</t>
+  </si>
+  <si>
+    <t>standardization of a variable by deviding it through its standard deviation, leading to a mean of 0 and a standard deviation of 1.</t>
+  </si>
+  <si>
+    <t>having multiple measurements per participant/object.</t>
+  </si>
+  <si>
+    <t>default behaviour of regression engines, giving the differences between groups compared to a reference group.</t>
+  </si>
+  <si>
+    <t>a method to deal with ordered factors, like a number of treatments.</t>
+  </si>
+  <si>
+    <t>A point of a graph where the slope is 0, usually with a change from rising to falling or the other way round.</t>
+  </si>
+  <si>
+    <t>a single value indicating the distribution of a value, calculated as the square root of variance.</t>
+  </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>squared standard deviation, a measure of the deviation of values from the mean.</t>
+  </si>
+  <si>
+    <t>if an effect cannot be further elevated, saturation occurs, e.g. effectiveness of painkillers cannot rise endlessly.</t>
+  </si>
+  <si>
+    <t>a way of transforming a variable such that the estimations and calculations are within the data range.</t>
+  </si>
+  <si>
+    <t>the difference between actual value and predicted value.</t>
+  </si>
+  <si>
+    <t>measuring the same aspect of a person/object multiple times, e.g. before and after treatment.</t>
+  </si>
+  <si>
+    <t>trying to achieve equal groups by letting chance decide which object/person ends up in which condition.</t>
+  </si>
+  <si>
+    <t>a serious of probabalistically determined steps.</t>
+  </si>
+  <si>
+    <t>variance in values that cannot be predicted with the model.</t>
+  </si>
+  <si>
+    <t>Comparing deviations of the grand mean.</t>
+  </si>
+  <si>
+    <t>A statistical test that works like an extended t-test, comparing multiple coefficients are differing from 0.</t>
+  </si>
+  <si>
+    <t>HPD</t>
+  </si>
+  <si>
+    <t>Random factor</t>
+  </si>
+  <si>
+    <t>a factor where levels are drawn from an overarching distribution, usually Gaussian.</t>
+  </si>
+  <si>
+    <t>Mixed-effects model</t>
+  </si>
+  <si>
+    <t>Random effect</t>
   </si>
 </sst>
 </file>
@@ -1507,10 +1594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D169"/>
+  <dimension ref="A1:D173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="B106" sqref="B106"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="A140" sqref="A140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1540,7 +1627,7 @@
         <v>205</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>203</v>
@@ -1551,21 +1638,21 @@
     </row>
     <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>292</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>50</v>
@@ -1576,7 +1663,7 @@
         <v>201</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>117</v>
@@ -1604,7 +1691,7 @@
         <v>242</v>
       </c>
       <c r="B7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C7" t="s">
         <v>53</v>
@@ -1612,10 +1699,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>300</v>
+      </c>
+      <c r="B8" t="s">
         <v>301</v>
-      </c>
-      <c r="B8" t="s">
-        <v>302</v>
       </c>
       <c r="C8" t="s">
         <v>213</v>
@@ -1626,7 +1713,7 @@
         <v>243</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C9" s="2">
         <v>3</v>
@@ -1665,7 +1752,7 @@
         <v>204</v>
       </c>
       <c r="B12" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C12" t="s">
         <v>203</v>
@@ -1690,13 +1777,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B14" t="s">
+        <v>344</v>
+      </c>
+      <c r="C14" t="s">
         <v>345</v>
-      </c>
-      <c r="C14" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -1704,7 +1791,7 @@
         <v>229</v>
       </c>
       <c r="B15" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C15" t="s">
         <v>193</v>
@@ -1715,13 +1802,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B16" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C16" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
@@ -1754,7 +1841,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B19" t="s">
         <v>104</v>
@@ -1782,10 +1869,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
+        <v>334</v>
+      </c>
+      <c r="B21" t="s">
         <v>335</v>
-      </c>
-      <c r="B21" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
@@ -1804,10 +1891,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>307</v>
+      </c>
+      <c r="B23" t="s">
         <v>308</v>
-      </c>
-      <c r="B23" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
@@ -1815,7 +1902,7 @@
         <v>206</v>
       </c>
       <c r="B24" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C24" t="s">
         <v>207</v>
@@ -1826,7 +1913,7 @@
         <v>197</v>
       </c>
       <c r="B25" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C25" t="s">
         <v>198</v>
@@ -1837,7 +1924,7 @@
         <v>199</v>
       </c>
       <c r="B26" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -1845,7 +1932,7 @@
         <v>191</v>
       </c>
       <c r="B27" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C27" t="s">
         <v>147</v>
@@ -1853,10 +1940,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B28" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
@@ -1875,10 +1962,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B30" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C30" s="2"/>
     </row>
@@ -1945,7 +2032,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>291</v>
+        <v>290</v>
+      </c>
+      <c r="B36" t="s">
+        <v>400</v>
       </c>
       <c r="C36" t="s">
         <v>207</v>
@@ -1978,10 +2068,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B39" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C39" s="2"/>
     </row>
@@ -2004,7 +2094,7 @@
         <v>202</v>
       </c>
       <c r="B41" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C41" t="s">
         <v>203</v>
@@ -2012,29 +2102,29 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B42" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
+        <v>309</v>
+      </c>
+      <c r="B43" t="s">
         <v>310</v>
-      </c>
-      <c r="B43" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
+        <v>280</v>
+      </c>
+      <c r="B44" t="s">
+        <v>356</v>
+      </c>
+      <c r="C44" t="s">
         <v>281</v>
-      </c>
-      <c r="B44" t="s">
-        <v>357</v>
-      </c>
-      <c r="C44" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
@@ -2053,36 +2143,36 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B46" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C46" s="2"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C47" s="2"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B48" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C48" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B49" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
@@ -2124,19 +2214,19 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B53" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D53" s="2"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
+        <v>361</v>
+      </c>
+      <c r="B54" t="s">
         <v>362</v>
-      </c>
-      <c r="B54" t="s">
-        <v>363</v>
       </c>
       <c r="C54" t="s">
         <v>211</v>
@@ -2145,13 +2235,16 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>279</v>
+        <v>278</v>
+      </c>
+      <c r="B55" t="s">
+        <v>401</v>
       </c>
       <c r="D55" s="2"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
@@ -2170,15 +2263,15 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
+        <v>259</v>
+      </c>
+      <c r="B58" t="s">
         <v>260</v>
-      </c>
-      <c r="B58" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
@@ -2186,7 +2279,7 @@
         <v>238</v>
       </c>
       <c r="B60" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
@@ -2205,7 +2298,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
@@ -2224,10 +2317,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
+        <v>251</v>
+      </c>
+      <c r="B64" t="s">
         <v>252</v>
-      </c>
-      <c r="B64" t="s">
-        <v>253</v>
       </c>
       <c r="C64" t="s">
         <v>249</v>
@@ -2238,292 +2331,286 @@
         <v>218</v>
       </c>
       <c r="B65" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>96</v>
-      </c>
-      <c r="B66" t="s">
-        <v>97</v>
-      </c>
-      <c r="C66" t="s">
-        <v>131</v>
-      </c>
-      <c r="D66" t="s">
-        <v>132</v>
+        <v>402</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>219</v>
+        <v>96</v>
+      </c>
+      <c r="B67" t="s">
+        <v>97</v>
+      </c>
+      <c r="C67" t="s">
+        <v>131</v>
+      </c>
+      <c r="D67" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>18</v>
-      </c>
-      <c r="B68" t="s">
-        <v>165</v>
-      </c>
-      <c r="C68" t="s">
-        <v>64</v>
-      </c>
-      <c r="D68" t="s">
-        <v>57</v>
+        <v>219</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>108</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>166</v>
+        <v>18</v>
+      </c>
+      <c r="B69" t="s">
+        <v>165</v>
       </c>
       <c r="C69" t="s">
-        <v>133</v>
+        <v>64</v>
       </c>
       <c r="D69" t="s">
-        <v>134</v>
+        <v>57</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>251</v>
+        <v>108</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>366</v>
+        <v>166</v>
+      </c>
+      <c r="C70" t="s">
+        <v>133</v>
+      </c>
+      <c r="D70" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>19</v>
+        <v>250</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C71" t="s">
-        <v>46</v>
-      </c>
-      <c r="D71" t="s">
-        <v>65</v>
+        <v>365</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>286</v>
+        <v>19</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>297</v>
+        <v>167</v>
       </c>
       <c r="C72" t="s">
-        <v>211</v>
+        <v>46</v>
+      </c>
+      <c r="D72" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>333</v>
+        <v>285</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C73" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>239</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>367</v>
+        <v>332</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>94</v>
+        <v>239</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="C75" t="s">
-        <v>131</v>
-      </c>
-      <c r="D75" t="s">
-        <v>135</v>
+        <v>366</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>20</v>
+        <v>94</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>168</v>
+        <v>185</v>
       </c>
       <c r="C76" t="s">
-        <v>49</v>
+        <v>131</v>
       </c>
       <c r="D76" t="s">
-        <v>66</v>
+        <v>135</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>21</v>
-      </c>
-      <c r="B77" t="s">
-        <v>41</v>
+        <v>20</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>168</v>
       </c>
       <c r="C77" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D77" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>256</v>
+        <v>21</v>
+      </c>
+      <c r="B78" t="s">
+        <v>41</v>
       </c>
       <c r="C78" t="s">
-        <v>258</v>
+        <v>55</v>
+      </c>
+      <c r="D78" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>230</v>
-      </c>
-      <c r="B79" t="s">
-        <v>368</v>
-      </c>
-      <c r="C79" s="2">
-        <v>5</v>
+        <v>255</v>
+      </c>
+      <c r="C79" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>210</v>
+        <v>230</v>
+      </c>
+      <c r="B80" t="s">
+        <v>367</v>
+      </c>
+      <c r="C80" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>334</v>
-      </c>
-      <c r="B81" t="s">
-        <v>370</v>
+        <v>210</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>275</v>
+        <v>333</v>
       </c>
       <c r="B82" t="s">
         <v>369</v>
       </c>
-      <c r="C82" t="s">
-        <v>147</v>
-      </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>68</v>
+        <v>274</v>
       </c>
       <c r="B83" t="s">
-        <v>169</v>
+        <v>368</v>
       </c>
       <c r="C83" t="s">
-        <v>46</v>
-      </c>
-      <c r="D83" t="s">
-        <v>69</v>
+        <v>147</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="B84" t="s">
-        <v>98</v>
+        <v>169</v>
       </c>
       <c r="C84" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="D84" t="s">
-        <v>136</v>
+        <v>69</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>332</v>
+        <v>99</v>
       </c>
       <c r="B85" t="s">
-        <v>371</v>
+        <v>98</v>
+      </c>
+      <c r="C85" t="s">
+        <v>59</v>
+      </c>
+      <c r="D85" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>314</v>
+        <v>331</v>
       </c>
       <c r="B86" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>263</v>
-      </c>
-      <c r="C87" t="s">
-        <v>258</v>
+        <v>313</v>
+      </c>
+      <c r="B87" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>109</v>
-      </c>
-      <c r="B88" t="s">
-        <v>171</v>
+        <v>262</v>
       </c>
       <c r="C88" t="s">
-        <v>137</v>
-      </c>
-      <c r="D88" t="s">
-        <v>138</v>
+        <v>257</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>225</v>
+        <v>109</v>
       </c>
       <c r="B89" t="s">
-        <v>373</v>
+        <v>171</v>
+      </c>
+      <c r="C89" t="s">
+        <v>137</v>
+      </c>
+      <c r="D89" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>83</v>
+        <v>225</v>
       </c>
       <c r="B90" t="s">
-        <v>262</v>
-      </c>
-      <c r="C90" t="s">
-        <v>139</v>
-      </c>
-      <c r="D90" t="s">
-        <v>140</v>
+        <v>372</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>244</v>
+        <v>83</v>
       </c>
       <c r="B91" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C91" t="s">
-        <v>249</v>
+        <v>139</v>
+      </c>
+      <c r="D91" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B92" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="C92" t="s">
         <v>249</v>
@@ -2531,53 +2618,47 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>277</v>
+        <v>246</v>
       </c>
       <c r="B93" t="s">
-        <v>374</v>
+        <v>269</v>
+      </c>
+      <c r="C93" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>226</v>
+        <v>276</v>
       </c>
       <c r="B94" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>306</v>
+        <v>226</v>
       </c>
       <c r="B95" t="s">
-        <v>307</v>
+        <v>374</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>245</v>
-      </c>
-      <c r="B96" t="s">
-        <v>268</v>
-      </c>
-      <c r="C96" t="s">
-        <v>249</v>
+        <v>405</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B97" t="s">
-        <v>304</v>
-      </c>
-      <c r="C97" t="s">
-        <v>213</v>
+        <v>306</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B98" t="s">
         <v>267</v>
@@ -2588,690 +2669,789 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>248</v>
+        <v>302</v>
+      </c>
+      <c r="B99" t="s">
+        <v>303</v>
       </c>
       <c r="C99" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>312</v>
+        <v>247</v>
       </c>
       <c r="B100" t="s">
-        <v>376</v>
+        <v>266</v>
+      </c>
+      <c r="C100" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>298</v>
-      </c>
-      <c r="B101" t="s">
-        <v>299</v>
+        <v>248</v>
+      </c>
+      <c r="C101" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>209</v>
+        <v>311</v>
       </c>
       <c r="B102" t="s">
-        <v>300</v>
+        <v>375</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B103" t="s">
-        <v>296</v>
-      </c>
-      <c r="C103" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>23</v>
+        <v>209</v>
       </c>
       <c r="B104" t="s">
-        <v>77</v>
-      </c>
-      <c r="C104" t="s">
-        <v>46</v>
-      </c>
-      <c r="D104" t="s">
-        <v>72</v>
+        <v>299</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>87</v>
+        <v>294</v>
       </c>
       <c r="B105" t="s">
-        <v>172</v>
+        <v>295</v>
       </c>
       <c r="C105" t="s">
-        <v>113</v>
-      </c>
-      <c r="D105" t="s">
-        <v>130</v>
+        <v>292</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>331</v>
+        <v>23</v>
+      </c>
+      <c r="B106" t="s">
+        <v>77</v>
+      </c>
+      <c r="C106" t="s">
+        <v>46</v>
+      </c>
+      <c r="D106" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>338</v>
+        <v>87</v>
       </c>
       <c r="B107" t="s">
-        <v>377</v>
+        <v>172</v>
+      </c>
+      <c r="C107" t="s">
+        <v>113</v>
+      </c>
+      <c r="D107" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>212</v>
-      </c>
-      <c r="B108" t="s">
-        <v>272</v>
-      </c>
-      <c r="C108" t="s">
-        <v>213</v>
+        <v>330</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>24</v>
+        <v>337</v>
       </c>
       <c r="B109" t="s">
-        <v>173</v>
-      </c>
-      <c r="C109" t="s">
-        <v>46</v>
-      </c>
-      <c r="D109" t="s">
-        <v>73</v>
+        <v>376</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>25</v>
+        <v>212</v>
       </c>
       <c r="B110" t="s">
-        <v>174</v>
+        <v>271</v>
       </c>
       <c r="C110" t="s">
-        <v>46</v>
-      </c>
-      <c r="D110" t="s">
-        <v>62</v>
+        <v>213</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>26</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>175</v>
+        <v>24</v>
+      </c>
+      <c r="B111" t="s">
+        <v>173</v>
       </c>
       <c r="C111" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D111" t="s">
-        <v>141</v>
+        <v>73</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>88</v>
+        <v>25</v>
       </c>
       <c r="B112" t="s">
-        <v>89</v>
+        <v>174</v>
       </c>
       <c r="C112" t="s">
-        <v>131</v>
+        <v>46</v>
       </c>
       <c r="D112" t="s">
-        <v>130</v>
+        <v>62</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>27</v>
-      </c>
-      <c r="B113" t="s">
-        <v>100</v>
+        <v>26</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="C113" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D113" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>28</v>
+        <v>88</v>
       </c>
       <c r="B114" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="C114" t="s">
-        <v>55</v>
+        <v>131</v>
       </c>
       <c r="D114" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>317</v>
+        <v>27</v>
+      </c>
+      <c r="B115" t="s">
+        <v>100</v>
+      </c>
+      <c r="C115" t="s">
+        <v>57</v>
+      </c>
+      <c r="D115" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="B116" t="s">
-        <v>81</v>
+        <v>42</v>
       </c>
       <c r="C116" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D116" t="s">
-        <v>62</v>
+        <v>143</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>273</v>
-      </c>
-      <c r="C117" t="s">
-        <v>139</v>
+        <v>316</v>
+      </c>
+      <c r="B117" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B118" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C118" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D118" t="s">
-        <v>144</v>
+        <v>62</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>278</v>
+        <v>272</v>
+      </c>
+      <c r="C119" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>29</v>
+        <v>90</v>
       </c>
       <c r="B120" t="s">
-        <v>176</v>
+        <v>91</v>
       </c>
       <c r="C120" t="s">
-        <v>127</v>
+        <v>46</v>
       </c>
       <c r="D120" t="s">
-        <v>62</v>
+        <v>144</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>82</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="C121" t="s">
-        <v>145</v>
-      </c>
-      <c r="D121" t="s">
-        <v>146</v>
+        <v>277</v>
+      </c>
+      <c r="B121" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B122" t="s">
-        <v>78</v>
+        <v>176</v>
       </c>
       <c r="C122" t="s">
-        <v>49</v>
+        <v>127</v>
       </c>
       <c r="D122" t="s">
-        <v>130</v>
+        <v>62</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>232</v>
+        <v>82</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C123" t="s">
+        <v>145</v>
+      </c>
+      <c r="D123" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>320</v>
+        <v>30</v>
+      </c>
+      <c r="B124" t="s">
+        <v>78</v>
+      </c>
+      <c r="C124" t="s">
+        <v>49</v>
+      </c>
+      <c r="D124" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>200</v>
+        <v>232</v>
+      </c>
+      <c r="B125" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>222</v>
+        <v>319</v>
+      </c>
+      <c r="B126" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>283</v>
+        <v>200</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>233</v>
-      </c>
-      <c r="B129" t="s">
-        <v>234</v>
+        <v>282</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>192</v>
-      </c>
-      <c r="C130" t="s">
-        <v>193</v>
+        <v>223</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>323</v>
+        <v>233</v>
       </c>
       <c r="B131" t="s">
-        <v>324</v>
+        <v>234</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>274</v>
+        <v>192</v>
+      </c>
+      <c r="B132" t="s">
+        <v>381</v>
+      </c>
+      <c r="C132" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>322</v>
       </c>
+      <c r="B133" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>215</v>
-      </c>
-      <c r="C135" t="s">
-        <v>216</v>
+        <v>321</v>
+      </c>
+      <c r="B135" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>214</v>
-      </c>
-      <c r="C136" t="s">
-        <v>213</v>
+        <v>270</v>
+      </c>
+      <c r="B136" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>250</v>
+        <v>215</v>
+      </c>
+      <c r="C137" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>31</v>
+        <v>214</v>
       </c>
       <c r="B138" t="s">
-        <v>43</v>
-      </c>
-      <c r="C138" s="2">
-        <v>4</v>
-      </c>
-      <c r="D138" t="s">
-        <v>62</v>
+        <v>384</v>
+      </c>
+      <c r="C138" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B139" t="s">
-        <v>44</v>
-      </c>
-      <c r="C139" t="s">
-        <v>55</v>
+        <v>43</v>
+      </c>
+      <c r="C139" s="2">
+        <v>4</v>
       </c>
       <c r="D139" t="s">
-        <v>137</v>
+        <v>62</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>257</v>
+        <v>32</v>
+      </c>
+      <c r="B140" t="s">
+        <v>44</v>
       </c>
       <c r="C140" t="s">
-        <v>258</v>
+        <v>55</v>
+      </c>
+      <c r="D140" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>195</v>
-      </c>
-      <c r="C141" s="2" t="s">
-        <v>139</v>
+        <v>406</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>325</v>
+        <v>403</v>
+      </c>
+      <c r="B142" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>287</v>
+        <v>256</v>
       </c>
       <c r="B143" t="s">
-        <v>289</v>
-      </c>
-      <c r="C143" s="2"/>
+        <v>399</v>
+      </c>
+      <c r="C143" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>105</v>
+        <v>195</v>
       </c>
       <c r="B144" t="s">
-        <v>178</v>
-      </c>
-      <c r="C144" t="s">
-        <v>147</v>
-      </c>
-      <c r="D144" t="s">
-        <v>62</v>
+        <v>398</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>106</v>
+        <v>324</v>
       </c>
       <c r="B145" t="s">
-        <v>179</v>
-      </c>
-      <c r="C145" t="s">
-        <v>148</v>
-      </c>
-      <c r="D145" t="s">
-        <v>149</v>
+        <v>397</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>107</v>
+        <v>286</v>
       </c>
       <c r="B146" t="s">
-        <v>180</v>
-      </c>
-      <c r="C146" t="s">
-        <v>148</v>
-      </c>
-      <c r="D146" t="s">
-        <v>150</v>
-      </c>
+        <v>288</v>
+      </c>
+      <c r="C146" s="2"/>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>319</v>
+        <v>105</v>
+      </c>
+      <c r="B147" t="s">
+        <v>178</v>
+      </c>
+      <c r="C147" t="s">
+        <v>147</v>
+      </c>
+      <c r="D147" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>235</v>
+        <v>106</v>
+      </c>
+      <c r="B148" t="s">
+        <v>179</v>
+      </c>
+      <c r="C148" t="s">
+        <v>148</v>
+      </c>
+      <c r="D148" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>181</v>
+        <v>107</v>
       </c>
       <c r="B149" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C149" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D149" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>329</v>
+        <v>318</v>
+      </c>
+      <c r="B150" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>33</v>
+        <v>235</v>
       </c>
       <c r="B151" t="s">
-        <v>183</v>
-      </c>
-      <c r="C151" t="s">
-        <v>49</v>
-      </c>
-      <c r="D151" t="s">
-        <v>153</v>
+        <v>395</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>194</v>
+        <v>181</v>
+      </c>
+      <c r="B152" t="s">
+        <v>182</v>
       </c>
       <c r="C152" t="s">
-        <v>193</v>
+        <v>151</v>
+      </c>
+      <c r="D152" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>189</v>
+        <v>328</v>
       </c>
       <c r="B153" t="s">
-        <v>190</v>
-      </c>
-      <c r="C153" t="s">
-        <v>147</v>
+        <v>393</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>196</v>
+        <v>33</v>
+      </c>
+      <c r="B154" t="s">
+        <v>183</v>
+      </c>
+      <c r="C154" t="s">
+        <v>49</v>
+      </c>
+      <c r="D154" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>224</v>
+        <v>194</v>
+      </c>
+      <c r="B155" t="s">
+        <v>394</v>
+      </c>
+      <c r="C155" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>34</v>
+        <v>189</v>
       </c>
       <c r="B156" t="s">
-        <v>79</v>
-      </c>
-      <c r="C156" s="2">
-        <v>1</v>
-      </c>
-      <c r="D156" t="s">
-        <v>136</v>
+        <v>190</v>
+      </c>
+      <c r="C156" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>35</v>
-      </c>
-      <c r="B157" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C157" s="2">
-        <v>4</v>
-      </c>
-      <c r="D157" t="s">
-        <v>154</v>
+        <v>196</v>
+      </c>
+      <c r="B157" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>326</v>
-      </c>
-      <c r="B158" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="C158" s="2"/>
+        <v>224</v>
+      </c>
+      <c r="B158" t="s">
+        <v>389</v>
+      </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>22</v>
-      </c>
-      <c r="B159" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="C159" t="s">
-        <v>70</v>
+        <v>34</v>
+      </c>
+      <c r="B159" t="s">
+        <v>79</v>
+      </c>
+      <c r="C159" s="2">
+        <v>1</v>
       </c>
       <c r="D159" t="s">
-        <v>71</v>
+        <v>136</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>208</v>
-      </c>
-      <c r="B160" s="3"/>
-      <c r="C160" s="2" t="s">
-        <v>207</v>
+        <v>35</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C160" s="2">
+        <v>4</v>
+      </c>
+      <c r="D160" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>36</v>
-      </c>
-      <c r="B161" t="s">
-        <v>45</v>
-      </c>
-      <c r="C161" s="2">
-        <v>4</v>
-      </c>
-      <c r="D161" t="s">
-        <v>155</v>
-      </c>
+        <v>325</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C161" s="2"/>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>95</v>
+        <v>22</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="C162" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="D162" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>240</v>
+        <v>208</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>241</v>
+        <v>388</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>112</v>
-      </c>
-      <c r="B164" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="C164" t="s">
-        <v>59</v>
+        <v>36</v>
+      </c>
+      <c r="B164" t="s">
+        <v>45</v>
+      </c>
+      <c r="C164" s="2">
+        <v>4</v>
       </c>
       <c r="D164" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>288</v>
-      </c>
-      <c r="B165" s="3"/>
+        <v>95</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C165" t="s">
+        <v>46</v>
+      </c>
+      <c r="D165" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>37</v>
-      </c>
-      <c r="B166" t="s">
-        <v>187</v>
-      </c>
-      <c r="C166" t="s">
-        <v>120</v>
-      </c>
-      <c r="D166" t="s">
-        <v>62</v>
+        <v>240</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>38</v>
-      </c>
-      <c r="B167" t="s">
-        <v>188</v>
+        <v>112</v>
+      </c>
+      <c r="B167" s="3" t="s">
+        <v>186</v>
       </c>
       <c r="C167" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D167" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>318</v>
+        <v>287</v>
+      </c>
+      <c r="B168" s="3" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>276</v>
+        <v>37</v>
+      </c>
+      <c r="B169" t="s">
+        <v>187</v>
+      </c>
+      <c r="C169" t="s">
+        <v>120</v>
+      </c>
+      <c r="D169" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A170" t="s">
+        <v>391</v>
+      </c>
+      <c r="B170" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A171" t="s">
+        <v>38</v>
+      </c>
+      <c r="B171" t="s">
+        <v>188</v>
+      </c>
+      <c r="C171" t="s">
+        <v>64</v>
+      </c>
+      <c r="D171" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A172" t="s">
+        <v>317</v>
+      </c>
+      <c r="B172" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A173" t="s">
+        <v>275</v>
+      </c>
+      <c r="B173" t="s">
+        <v>385</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D169">
-    <sortCondition ref="A138"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D173">
+    <sortCondition ref="A139"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
6, second round, until line 229
</commit_message>
<xml_diff>
--- a/Index_of_terms.xlsx
+++ b/Index_of_terms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steffi\Documents\work\schmettow\GitHub\New_Stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1AFBA8-32FD-4B00-A7F1-26EBEA1B9D50}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB995B9A-B6F3-43A8-B1FE-110F94F625D0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="419">
   <si>
     <t>Term</t>
   </si>
@@ -1274,6 +1274,33 @@
   </si>
   <si>
     <t>a fixed effect is a factor where levels are regarded so unsimilar, that the factor-level distribution can be practically considered infinite</t>
+  </si>
+  <si>
+    <t>Psychometrics</t>
+  </si>
+  <si>
+    <t>Distribution</t>
+  </si>
+  <si>
+    <t>Shrinkage</t>
+  </si>
+  <si>
+    <t>Linear effects model</t>
+  </si>
+  <si>
+    <t>Stroop</t>
+  </si>
+  <si>
+    <t>Reductionism</t>
+  </si>
+  <si>
+    <t>individual levels of random factors.</t>
+  </si>
+  <si>
+    <t>Random factor variation</t>
+  </si>
+  <si>
+    <t>Between-subject design</t>
   </si>
 </sst>
 </file>
@@ -1604,10 +1631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D175"/>
+  <dimension ref="A1:D183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0">
-      <selection activeCell="B175" sqref="B175"/>
+    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="B185" sqref="B185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1731,1750 +1758,1793 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" t="s">
-        <v>50</v>
+        <v>418</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>204</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>343</v>
+        <v>75</v>
       </c>
       <c r="C12" t="s">
-        <v>203</v>
+        <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>130</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>204</v>
       </c>
       <c r="B13" t="s">
-        <v>115</v>
+        <v>343</v>
       </c>
       <c r="C13" t="s">
-        <v>113</v>
+        <v>203</v>
       </c>
       <c r="D13" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>314</v>
+        <v>86</v>
       </c>
       <c r="B14" t="s">
-        <v>344</v>
+        <v>115</v>
       </c>
       <c r="C14" t="s">
-        <v>345</v>
+        <v>113</v>
+      </c>
+      <c r="D14" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>229</v>
+        <v>314</v>
       </c>
       <c r="B15" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C15" t="s">
-        <v>193</v>
-      </c>
-      <c r="D15" t="s">
-        <v>130</v>
+        <v>345</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>254</v>
+        <v>229</v>
       </c>
       <c r="B16" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C16" t="s">
-        <v>347</v>
+        <v>193</v>
+      </c>
+      <c r="D16" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>254</v>
       </c>
       <c r="B17" t="s">
-        <v>116</v>
+        <v>348</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" t="s">
-        <v>51</v>
+        <v>347</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D18" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>253</v>
+        <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="C19" t="s">
-        <v>117</v>
+        <v>53</v>
       </c>
       <c r="D19" t="s">
-        <v>118</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>110</v>
+        <v>253</v>
       </c>
       <c r="B20" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="C20" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D20" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>334</v>
+        <v>110</v>
       </c>
       <c r="B21" t="s">
-        <v>335</v>
+        <v>122</v>
+      </c>
+      <c r="C21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>334</v>
       </c>
       <c r="B22" t="s">
-        <v>158</v>
-      </c>
-      <c r="C22" t="s">
-        <v>55</v>
-      </c>
-      <c r="D22" t="s">
-        <v>56</v>
+        <v>335</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>307</v>
+        <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>308</v>
+        <v>158</v>
+      </c>
+      <c r="C23" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>206</v>
+        <v>307</v>
       </c>
       <c r="B24" t="s">
-        <v>289</v>
-      </c>
-      <c r="C24" t="s">
-        <v>207</v>
+        <v>308</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="B25" t="s">
-        <v>349</v>
+        <v>289</v>
       </c>
       <c r="C25" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B26" t="s">
-        <v>350</v>
+        <v>349</v>
+      </c>
+      <c r="C26" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="B27" t="s">
-        <v>351</v>
-      </c>
-      <c r="C27" t="s">
-        <v>147</v>
+        <v>350</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>320</v>
+        <v>191</v>
       </c>
       <c r="B28" t="s">
-        <v>352</v>
+        <v>351</v>
+      </c>
+      <c r="C28" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>320</v>
       </c>
       <c r="B29" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="2">
-        <v>4</v>
-      </c>
-      <c r="D29" t="s">
-        <v>52</v>
+        <v>352</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>264</v>
+        <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>353</v>
-      </c>
-      <c r="C30" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="C30" s="2">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>217</v>
-      </c>
+        <v>264</v>
+      </c>
+      <c r="B31" t="s">
+        <v>353</v>
+      </c>
+      <c r="C31" s="2"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>11</v>
-      </c>
-      <c r="B32" t="s">
-        <v>159</v>
-      </c>
-      <c r="C32" t="s">
-        <v>57</v>
-      </c>
-      <c r="D32" t="s">
-        <v>58</v>
+        <v>217</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B33" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C33" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D33" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>84</v>
+        <v>12</v>
       </c>
       <c r="B34" t="s">
-        <v>85</v>
+        <v>160</v>
       </c>
       <c r="C34" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D34" t="s">
-        <v>123</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B35" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C35" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="D35" t="s">
-        <v>62</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>290</v>
+        <v>92</v>
       </c>
       <c r="B36" t="s">
-        <v>400</v>
+        <v>93</v>
       </c>
       <c r="C36" t="s">
-        <v>207</v>
+        <v>46</v>
+      </c>
+      <c r="D36" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>13</v>
+        <v>290</v>
       </c>
       <c r="B37" t="s">
-        <v>76</v>
+        <v>400</v>
       </c>
       <c r="C37" t="s">
-        <v>46</v>
-      </c>
-      <c r="D37" t="s">
-        <v>124</v>
+        <v>207</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>220</v>
+        <v>13</v>
       </c>
       <c r="B38" t="s">
-        <v>221</v>
-      </c>
-      <c r="C38" s="2">
-        <v>5</v>
+        <v>76</v>
+      </c>
+      <c r="C38" t="s">
+        <v>46</v>
+      </c>
+      <c r="D38" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>329</v>
+        <v>220</v>
       </c>
       <c r="B39" t="s">
-        <v>354</v>
-      </c>
-      <c r="C39" s="2"/>
+        <v>221</v>
+      </c>
+      <c r="C39" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>111</v>
+        <v>329</v>
       </c>
       <c r="B40" t="s">
-        <v>161</v>
-      </c>
-      <c r="C40" t="s">
-        <v>126</v>
-      </c>
-      <c r="D40" t="s">
-        <v>125</v>
-      </c>
+        <v>354</v>
+      </c>
+      <c r="C40" s="2"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>202</v>
-      </c>
-      <c r="B41" t="s">
-        <v>284</v>
-      </c>
-      <c r="C41" t="s">
-        <v>203</v>
+        <v>411</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>315</v>
+        <v>111</v>
       </c>
       <c r="B42" t="s">
-        <v>355</v>
+        <v>161</v>
+      </c>
+      <c r="C42" t="s">
+        <v>126</v>
+      </c>
+      <c r="D42" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>309</v>
+        <v>202</v>
       </c>
       <c r="B43" t="s">
-        <v>310</v>
+        <v>284</v>
+      </c>
+      <c r="C43" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>280</v>
+        <v>315</v>
       </c>
       <c r="B44" t="s">
-        <v>356</v>
-      </c>
-      <c r="C44" t="s">
-        <v>281</v>
+        <v>355</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>14</v>
+        <v>309</v>
       </c>
       <c r="B45" t="s">
-        <v>101</v>
-      </c>
-      <c r="C45" s="2">
-        <v>4</v>
-      </c>
-      <c r="D45" t="s">
-        <v>61</v>
+        <v>310</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
       <c r="B46" t="s">
-        <v>357</v>
-      </c>
-      <c r="C46" s="2"/>
+        <v>356</v>
+      </c>
+      <c r="C46" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>279</v>
-      </c>
-      <c r="C47" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="B47" t="s">
+        <v>101</v>
+      </c>
+      <c r="C47" s="2">
+        <v>4</v>
+      </c>
+      <c r="D47" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="B48" t="s">
-        <v>358</v>
-      </c>
-      <c r="C48" t="s">
-        <v>257</v>
-      </c>
+        <v>357</v>
+      </c>
+      <c r="C48" s="2"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>312</v>
-      </c>
-      <c r="B49" t="s">
-        <v>359</v>
-      </c>
+        <v>279</v>
+      </c>
+      <c r="C49" s="2"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>236</v>
+        <v>258</v>
       </c>
       <c r="B50" t="s">
-        <v>237</v>
-      </c>
-      <c r="C50" s="2"/>
+        <v>358</v>
+      </c>
+      <c r="C50" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>103</v>
+        <v>312</v>
       </c>
       <c r="B51" t="s">
-        <v>102</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D51" t="s">
-        <v>128</v>
+        <v>359</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>15</v>
+        <v>236</v>
       </c>
       <c r="B52" t="s">
-        <v>162</v>
-      </c>
-      <c r="C52" t="s">
-        <v>46</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>62</v>
-      </c>
+        <v>237</v>
+      </c>
+      <c r="C52" s="2"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>283</v>
+        <v>103</v>
       </c>
       <c r="B53" t="s">
-        <v>360</v>
-      </c>
-      <c r="D53" s="2"/>
+        <v>102</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D53" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>361</v>
+        <v>15</v>
       </c>
       <c r="B54" t="s">
-        <v>362</v>
+        <v>162</v>
       </c>
       <c r="C54" t="s">
-        <v>211</v>
-      </c>
-      <c r="D54" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="B55" t="s">
-        <v>401</v>
+        <v>360</v>
       </c>
       <c r="D55" s="2"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>336</v>
-      </c>
+        <v>361</v>
+      </c>
+      <c r="B56" t="s">
+        <v>362</v>
+      </c>
+      <c r="C56" t="s">
+        <v>211</v>
+      </c>
+      <c r="D56" s="2"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>16</v>
+        <v>408</v>
       </c>
       <c r="B57" t="s">
-        <v>40</v>
-      </c>
-      <c r="C57" t="s">
-        <v>63</v>
-      </c>
-      <c r="D57" t="s">
-        <v>62</v>
+        <v>409</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>259</v>
+        <v>278</v>
       </c>
       <c r="B58" t="s">
-        <v>260</v>
-      </c>
+        <v>401</v>
+      </c>
+      <c r="D58" s="2"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>304</v>
+        <v>336</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>238</v>
+        <v>16</v>
       </c>
       <c r="B60" t="s">
-        <v>363</v>
+        <v>40</v>
+      </c>
+      <c r="C60" t="s">
+        <v>63</v>
+      </c>
+      <c r="D60" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>231</v>
+        <v>259</v>
       </c>
       <c r="B61" t="s">
-        <v>163</v>
-      </c>
-      <c r="C61" t="s">
-        <v>53</v>
-      </c>
-      <c r="D61" t="s">
-        <v>129</v>
+        <v>260</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>268</v>
+        <v>304</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>17</v>
+        <v>238</v>
       </c>
       <c r="B63" t="s">
-        <v>164</v>
-      </c>
-      <c r="C63" t="s">
-        <v>63</v>
-      </c>
-      <c r="D63" t="s">
-        <v>130</v>
+        <v>363</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>251</v>
+        <v>231</v>
       </c>
       <c r="B64" t="s">
-        <v>252</v>
+        <v>163</v>
       </c>
       <c r="C64" t="s">
-        <v>249</v>
+        <v>53</v>
+      </c>
+      <c r="D64" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>218</v>
-      </c>
-      <c r="B65" t="s">
-        <v>364</v>
+        <v>268</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>402</v>
+        <v>17</v>
+      </c>
+      <c r="B66" t="s">
+        <v>164</v>
+      </c>
+      <c r="C66" t="s">
+        <v>63</v>
+      </c>
+      <c r="D66" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>96</v>
+        <v>251</v>
       </c>
       <c r="B67" t="s">
-        <v>97</v>
+        <v>252</v>
       </c>
       <c r="C67" t="s">
-        <v>131</v>
-      </c>
-      <c r="D67" t="s">
-        <v>132</v>
+        <v>249</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>219</v>
+        <v>218</v>
+      </c>
+      <c r="B68" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>18</v>
-      </c>
-      <c r="B69" t="s">
-        <v>165</v>
-      </c>
-      <c r="C69" t="s">
-        <v>64</v>
-      </c>
-      <c r="D69" t="s">
-        <v>57</v>
+        <v>402</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>108</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>166</v>
+        <v>96</v>
+      </c>
+      <c r="B70" t="s">
+        <v>97</v>
       </c>
       <c r="C70" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D70" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>250</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>365</v>
+        <v>219</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>19</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>167</v>
+        <v>18</v>
+      </c>
+      <c r="B72" t="s">
+        <v>165</v>
       </c>
       <c r="C72" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="D72" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>285</v>
+        <v>108</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>296</v>
+        <v>166</v>
       </c>
       <c r="C73" t="s">
-        <v>211</v>
+        <v>133</v>
+      </c>
+      <c r="D73" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>332</v>
+        <v>250</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>239</v>
+        <v>19</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>366</v>
+        <v>167</v>
+      </c>
+      <c r="C75" t="s">
+        <v>46</v>
+      </c>
+      <c r="D75" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>94</v>
+        <v>285</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>185</v>
+        <v>296</v>
       </c>
       <c r="C76" t="s">
-        <v>131</v>
-      </c>
-      <c r="D76" t="s">
-        <v>135</v>
+        <v>211</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>20</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C77" t="s">
-        <v>49</v>
-      </c>
-      <c r="D77" t="s">
-        <v>66</v>
+        <v>332</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>21</v>
-      </c>
-      <c r="B78" t="s">
-        <v>41</v>
-      </c>
-      <c r="C78" t="s">
-        <v>55</v>
-      </c>
-      <c r="D78" t="s">
-        <v>67</v>
+        <v>239</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>255</v>
+        <v>94</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>185</v>
       </c>
       <c r="C79" t="s">
-        <v>257</v>
+        <v>131</v>
+      </c>
+      <c r="D79" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>230</v>
-      </c>
-      <c r="B80" t="s">
-        <v>367</v>
-      </c>
-      <c r="C80" s="2">
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C80" t="s">
+        <v>49</v>
+      </c>
+      <c r="D80" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>210</v>
+        <v>21</v>
+      </c>
+      <c r="B81" t="s">
+        <v>41</v>
+      </c>
+      <c r="C81" t="s">
+        <v>55</v>
+      </c>
+      <c r="D81" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>333</v>
-      </c>
-      <c r="B82" t="s">
-        <v>369</v>
+        <v>255</v>
+      </c>
+      <c r="C82" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>274</v>
-      </c>
-      <c r="B83" t="s">
-        <v>368</v>
-      </c>
-      <c r="C83" t="s">
-        <v>147</v>
+        <v>413</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>68</v>
+        <v>230</v>
       </c>
       <c r="B84" t="s">
-        <v>169</v>
-      </c>
-      <c r="C84" t="s">
-        <v>46</v>
-      </c>
-      <c r="D84" t="s">
-        <v>69</v>
+        <v>367</v>
+      </c>
+      <c r="C84" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>99</v>
-      </c>
-      <c r="B85" t="s">
-        <v>98</v>
-      </c>
-      <c r="C85" t="s">
-        <v>59</v>
-      </c>
-      <c r="D85" t="s">
-        <v>136</v>
+        <v>210</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B86" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>313</v>
+        <v>274</v>
       </c>
       <c r="B87" t="s">
-        <v>371</v>
+        <v>368</v>
+      </c>
+      <c r="C87" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>262</v>
+        <v>68</v>
+      </c>
+      <c r="B88" t="s">
+        <v>169</v>
       </c>
       <c r="C88" t="s">
-        <v>257</v>
+        <v>46</v>
+      </c>
+      <c r="D88" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="B89" t="s">
-        <v>171</v>
+        <v>98</v>
       </c>
       <c r="C89" t="s">
-        <v>137</v>
+        <v>59</v>
       </c>
       <c r="D89" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>225</v>
+        <v>331</v>
       </c>
       <c r="B90" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>83</v>
+        <v>313</v>
       </c>
       <c r="B91" t="s">
-        <v>261</v>
-      </c>
-      <c r="C91" t="s">
-        <v>139</v>
-      </c>
-      <c r="D91" t="s">
-        <v>140</v>
+        <v>371</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>244</v>
-      </c>
-      <c r="B92" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C92" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>246</v>
+        <v>109</v>
       </c>
       <c r="B93" t="s">
-        <v>269</v>
+        <v>171</v>
       </c>
       <c r="C93" t="s">
-        <v>249</v>
+        <v>137</v>
+      </c>
+      <c r="D93" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>276</v>
+        <v>225</v>
       </c>
       <c r="B94" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>226</v>
+        <v>83</v>
       </c>
       <c r="B95" t="s">
-        <v>374</v>
+        <v>261</v>
+      </c>
+      <c r="C95" t="s">
+        <v>139</v>
+      </c>
+      <c r="D95" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>405</v>
+        <v>244</v>
+      </c>
+      <c r="B96" t="s">
+        <v>265</v>
+      </c>
+      <c r="C96" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>305</v>
+        <v>246</v>
       </c>
       <c r="B97" t="s">
-        <v>306</v>
+        <v>269</v>
+      </c>
+      <c r="C97" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>245</v>
+        <v>276</v>
       </c>
       <c r="B98" t="s">
-        <v>267</v>
-      </c>
-      <c r="C98" t="s">
-        <v>249</v>
+        <v>373</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>302</v>
+        <v>226</v>
       </c>
       <c r="B99" t="s">
-        <v>303</v>
-      </c>
-      <c r="C99" t="s">
-        <v>213</v>
+        <v>374</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>247</v>
-      </c>
-      <c r="B100" t="s">
-        <v>266</v>
-      </c>
-      <c r="C100" t="s">
-        <v>249</v>
+        <v>405</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>248</v>
-      </c>
-      <c r="C101" t="s">
-        <v>249</v>
+        <v>305</v>
+      </c>
+      <c r="B101" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>311</v>
+        <v>245</v>
       </c>
       <c r="B102" t="s">
-        <v>375</v>
+        <v>267</v>
+      </c>
+      <c r="C102" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="B103" t="s">
-        <v>298</v>
+        <v>303</v>
+      </c>
+      <c r="C103" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>209</v>
+        <v>247</v>
       </c>
       <c r="B104" t="s">
-        <v>299</v>
+        <v>266</v>
+      </c>
+      <c r="C104" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>294</v>
-      </c>
-      <c r="B105" t="s">
-        <v>295</v>
+        <v>248</v>
       </c>
       <c r="C105" t="s">
-        <v>292</v>
+        <v>249</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>23</v>
+        <v>311</v>
       </c>
       <c r="B106" t="s">
-        <v>77</v>
-      </c>
-      <c r="C106" t="s">
-        <v>46</v>
-      </c>
-      <c r="D106" t="s">
-        <v>72</v>
+        <v>375</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>87</v>
+        <v>297</v>
       </c>
       <c r="B107" t="s">
-        <v>172</v>
-      </c>
-      <c r="C107" t="s">
-        <v>113</v>
-      </c>
-      <c r="D107" t="s">
-        <v>130</v>
+        <v>298</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>330</v>
+        <v>209</v>
+      </c>
+      <c r="B108" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>337</v>
+        <v>294</v>
       </c>
       <c r="B109" t="s">
-        <v>376</v>
+        <v>295</v>
+      </c>
+      <c r="C109" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>212</v>
+        <v>23</v>
       </c>
       <c r="B110" t="s">
-        <v>271</v>
+        <v>77</v>
       </c>
       <c r="C110" t="s">
-        <v>213</v>
+        <v>46</v>
+      </c>
+      <c r="D110" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>24</v>
+        <v>87</v>
       </c>
       <c r="B111" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C111" t="s">
-        <v>46</v>
+        <v>113</v>
       </c>
       <c r="D111" t="s">
-        <v>73</v>
+        <v>130</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>25</v>
-      </c>
-      <c r="B112" t="s">
-        <v>174</v>
-      </c>
-      <c r="C112" t="s">
-        <v>46</v>
-      </c>
-      <c r="D112" t="s">
-        <v>62</v>
+        <v>407</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>26</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C113" t="s">
-        <v>49</v>
-      </c>
-      <c r="D113" t="s">
-        <v>141</v>
+        <v>330</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>88</v>
+        <v>337</v>
       </c>
       <c r="B114" t="s">
-        <v>89</v>
-      </c>
-      <c r="C114" t="s">
-        <v>131</v>
-      </c>
-      <c r="D114" t="s">
-        <v>130</v>
+        <v>376</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>27</v>
+        <v>212</v>
       </c>
       <c r="B115" t="s">
-        <v>100</v>
+        <v>271</v>
       </c>
       <c r="C115" t="s">
-        <v>57</v>
-      </c>
-      <c r="D115" t="s">
-        <v>142</v>
+        <v>213</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B116" t="s">
-        <v>42</v>
+        <v>173</v>
       </c>
       <c r="C116" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D116" t="s">
-        <v>143</v>
+        <v>73</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>316</v>
+        <v>25</v>
       </c>
       <c r="B117" t="s">
-        <v>377</v>
+        <v>174</v>
+      </c>
+      <c r="C117" t="s">
+        <v>46</v>
+      </c>
+      <c r="D117" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>80</v>
-      </c>
-      <c r="B118" t="s">
-        <v>81</v>
+        <v>26</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="C118" t="s">
         <v>49</v>
       </c>
       <c r="D118" t="s">
-        <v>62</v>
+        <v>141</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>272</v>
+        <v>88</v>
+      </c>
+      <c r="B119" t="s">
+        <v>89</v>
       </c>
       <c r="C119" t="s">
-        <v>139</v>
+        <v>131</v>
+      </c>
+      <c r="D119" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>90</v>
+        <v>27</v>
       </c>
       <c r="B120" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="C120" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="D120" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>277</v>
+        <v>28</v>
       </c>
       <c r="B121" t="s">
-        <v>378</v>
+        <v>42</v>
+      </c>
+      <c r="C121" t="s">
+        <v>55</v>
+      </c>
+      <c r="D121" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>29</v>
+        <v>316</v>
       </c>
       <c r="B122" t="s">
-        <v>176</v>
-      </c>
-      <c r="C122" t="s">
-        <v>127</v>
-      </c>
-      <c r="D122" t="s">
-        <v>62</v>
+        <v>377</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>82</v>
-      </c>
-      <c r="B123" s="3" t="s">
-        <v>177</v>
+        <v>80</v>
+      </c>
+      <c r="B123" t="s">
+        <v>81</v>
       </c>
       <c r="C123" t="s">
-        <v>145</v>
+        <v>49</v>
       </c>
       <c r="D123" t="s">
-        <v>146</v>
+        <v>62</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>30</v>
-      </c>
-      <c r="B124" t="s">
-        <v>78</v>
+        <v>272</v>
       </c>
       <c r="C124" t="s">
-        <v>49</v>
-      </c>
-      <c r="D124" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>232</v>
+        <v>90</v>
       </c>
       <c r="B125" t="s">
-        <v>379</v>
+        <v>91</v>
+      </c>
+      <c r="C125" t="s">
+        <v>46</v>
+      </c>
+      <c r="D125" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>319</v>
+        <v>277</v>
       </c>
       <c r="B126" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>200</v>
+        <v>29</v>
+      </c>
+      <c r="B127" t="s">
+        <v>176</v>
+      </c>
+      <c r="C127" t="s">
+        <v>127</v>
+      </c>
+      <c r="D127" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>222</v>
+        <v>82</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C128" t="s">
+        <v>145</v>
+      </c>
+      <c r="D128" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>282</v>
+        <v>30</v>
+      </c>
+      <c r="B129" t="s">
+        <v>78</v>
+      </c>
+      <c r="C129" t="s">
+        <v>49</v>
+      </c>
+      <c r="D129" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>223</v>
+        <v>232</v>
+      </c>
+      <c r="B130" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>233</v>
+        <v>319</v>
       </c>
       <c r="B131" t="s">
-        <v>234</v>
+        <v>380</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>192</v>
-      </c>
-      <c r="B132" t="s">
-        <v>381</v>
-      </c>
-      <c r="C132" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>322</v>
-      </c>
-      <c r="B133" t="s">
-        <v>323</v>
+        <v>222</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>321</v>
-      </c>
-      <c r="B135" t="s">
-        <v>382</v>
+        <v>223</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>270</v>
+        <v>233</v>
       </c>
       <c r="B136" t="s">
-        <v>383</v>
+        <v>234</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>215</v>
+        <v>192</v>
+      </c>
+      <c r="B137" t="s">
+        <v>381</v>
       </c>
       <c r="C137" t="s">
-        <v>216</v>
+        <v>193</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>214</v>
+        <v>322</v>
       </c>
       <c r="B138" t="s">
-        <v>384</v>
-      </c>
-      <c r="C138" t="s">
-        <v>213</v>
+        <v>323</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>31</v>
-      </c>
-      <c r="B139" t="s">
-        <v>43</v>
-      </c>
-      <c r="C139" s="2">
-        <v>4</v>
-      </c>
-      <c r="D139" t="s">
-        <v>62</v>
+        <v>273</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>32</v>
+        <v>321</v>
       </c>
       <c r="B140" t="s">
-        <v>44</v>
-      </c>
-      <c r="C140" t="s">
-        <v>55</v>
-      </c>
-      <c r="D140" t="s">
-        <v>137</v>
+        <v>382</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>403</v>
+        <v>270</v>
       </c>
       <c r="B142" t="s">
-        <v>404</v>
+        <v>383</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>256</v>
-      </c>
-      <c r="B143" t="s">
-        <v>399</v>
+        <v>215</v>
       </c>
       <c r="C143" t="s">
-        <v>257</v>
+        <v>216</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>195</v>
+        <v>214</v>
       </c>
       <c r="B144" t="s">
-        <v>398</v>
-      </c>
-      <c r="C144" s="2" t="s">
-        <v>139</v>
+        <v>384</v>
+      </c>
+      <c r="C144" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>324</v>
+        <v>31</v>
       </c>
       <c r="B145" t="s">
-        <v>397</v>
+        <v>43</v>
+      </c>
+      <c r="C145" s="2">
+        <v>4</v>
+      </c>
+      <c r="D145" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>286</v>
+        <v>32</v>
       </c>
       <c r="B146" t="s">
-        <v>288</v>
-      </c>
-      <c r="C146" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="C146" t="s">
+        <v>55</v>
+      </c>
+      <c r="D146" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>105</v>
+        <v>406</v>
       </c>
       <c r="B147" t="s">
-        <v>178</v>
-      </c>
-      <c r="C147" t="s">
-        <v>147</v>
-      </c>
-      <c r="D147" t="s">
-        <v>62</v>
+        <v>416</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>106</v>
+        <v>403</v>
       </c>
       <c r="B148" t="s">
-        <v>179</v>
-      </c>
-      <c r="C148" t="s">
-        <v>148</v>
-      </c>
-      <c r="D148" t="s">
-        <v>149</v>
+        <v>404</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>107</v>
-      </c>
-      <c r="B149" t="s">
-        <v>180</v>
-      </c>
-      <c r="C149" t="s">
-        <v>148</v>
-      </c>
-      <c r="D149" t="s">
-        <v>150</v>
+        <v>417</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>318</v>
+        <v>256</v>
       </c>
       <c r="B150" t="s">
-        <v>396</v>
+        <v>399</v>
+      </c>
+      <c r="C150" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>235</v>
+        <v>195</v>
       </c>
       <c r="B151" t="s">
-        <v>395</v>
+        <v>398</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>181</v>
+        <v>324</v>
       </c>
       <c r="B152" t="s">
-        <v>182</v>
-      </c>
-      <c r="C152" t="s">
-        <v>151</v>
-      </c>
-      <c r="D152" t="s">
-        <v>152</v>
+        <v>397</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>328</v>
-      </c>
-      <c r="B153" t="s">
-        <v>393</v>
+        <v>415</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>33</v>
+        <v>286</v>
       </c>
       <c r="B154" t="s">
-        <v>183</v>
-      </c>
-      <c r="C154" t="s">
-        <v>49</v>
-      </c>
-      <c r="D154" t="s">
-        <v>153</v>
-      </c>
+        <v>288</v>
+      </c>
+      <c r="C154" s="2"/>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>194</v>
+        <v>105</v>
       </c>
       <c r="B155" t="s">
-        <v>394</v>
+        <v>178</v>
       </c>
       <c r="C155" t="s">
-        <v>193</v>
+        <v>147</v>
+      </c>
+      <c r="D155" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>189</v>
+        <v>106</v>
       </c>
       <c r="B156" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="C156" t="s">
-        <v>147</v>
+        <v>148</v>
+      </c>
+      <c r="D156" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>196</v>
+        <v>107</v>
       </c>
       <c r="B157" t="s">
-        <v>390</v>
+        <v>180</v>
+      </c>
+      <c r="C157" t="s">
+        <v>148</v>
+      </c>
+      <c r="D157" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>224</v>
+        <v>318</v>
       </c>
       <c r="B158" t="s">
-        <v>389</v>
+        <v>396</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>34</v>
+        <v>235</v>
       </c>
       <c r="B159" t="s">
-        <v>79</v>
-      </c>
-      <c r="C159" s="2">
-        <v>1</v>
-      </c>
-      <c r="D159" t="s">
-        <v>136</v>
+        <v>395</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>35</v>
-      </c>
-      <c r="B160" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C160" s="2">
-        <v>4</v>
+        <v>181</v>
+      </c>
+      <c r="B160" t="s">
+        <v>182</v>
+      </c>
+      <c r="C160" t="s">
+        <v>151</v>
       </c>
       <c r="D160" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>325</v>
-      </c>
-      <c r="B161" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="C161" s="2"/>
+        <v>328</v>
+      </c>
+      <c r="B161" t="s">
+        <v>393</v>
+      </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>22</v>
-      </c>
-      <c r="B162" s="3" t="s">
-        <v>170</v>
+        <v>33</v>
+      </c>
+      <c r="B162" t="s">
+        <v>183</v>
       </c>
       <c r="C162" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="D162" t="s">
-        <v>71</v>
+        <v>153</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>208</v>
-      </c>
-      <c r="B163" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="C163" s="2" t="s">
-        <v>207</v>
+        <v>194</v>
+      </c>
+      <c r="B163" t="s">
+        <v>394</v>
+      </c>
+      <c r="C163" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>36</v>
-      </c>
-      <c r="B164" t="s">
-        <v>45</v>
-      </c>
-      <c r="C164" s="2">
-        <v>4</v>
-      </c>
-      <c r="D164" t="s">
-        <v>155</v>
+        <v>412</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>95</v>
-      </c>
-      <c r="B165" s="3" t="s">
-        <v>185</v>
+        <v>189</v>
+      </c>
+      <c r="B165" t="s">
+        <v>190</v>
       </c>
       <c r="C165" t="s">
-        <v>46</v>
-      </c>
-      <c r="D165" t="s">
-        <v>62</v>
+        <v>147</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>240</v>
-      </c>
-      <c r="B166" s="3" t="s">
-        <v>241</v>
+        <v>196</v>
+      </c>
+      <c r="B166" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>112</v>
-      </c>
-      <c r="B167" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="C167" t="s">
-        <v>59</v>
-      </c>
-      <c r="D167" t="s">
-        <v>156</v>
+        <v>224</v>
+      </c>
+      <c r="B167" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>287</v>
-      </c>
-      <c r="B168" s="3" t="s">
-        <v>387</v>
+        <v>34</v>
+      </c>
+      <c r="B168" t="s">
+        <v>79</v>
+      </c>
+      <c r="C168" s="2">
+        <v>1</v>
+      </c>
+      <c r="D168" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>37</v>
-      </c>
-      <c r="B169" t="s">
-        <v>187</v>
-      </c>
-      <c r="C169" t="s">
-        <v>120</v>
+        <v>35</v>
+      </c>
+      <c r="B169" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C169" s="2">
+        <v>4</v>
       </c>
       <c r="D169" t="s">
-        <v>62</v>
+        <v>154</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>391</v>
-      </c>
-      <c r="B170" t="s">
-        <v>392</v>
-      </c>
+        <v>325</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C170" s="2"/>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>38</v>
-      </c>
-      <c r="B171" t="s">
-        <v>188</v>
+        <v>22</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>170</v>
       </c>
       <c r="C171" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D171" t="s">
-        <v>157</v>
+        <v>71</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>317</v>
-      </c>
-      <c r="B172" t="s">
-        <v>386</v>
+        <v>414</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>275</v>
-      </c>
-      <c r="B173" t="s">
-        <v>385</v>
+        <v>208</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C173" s="2" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>407</v>
+        <v>36</v>
+      </c>
+      <c r="B174" t="s">
+        <v>45</v>
+      </c>
+      <c r="C174" s="2">
+        <v>4</v>
+      </c>
+      <c r="D174" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>408</v>
-      </c>
-      <c r="B175" t="s">
-        <v>409</v>
+        <v>95</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C175" t="s">
+        <v>46</v>
+      </c>
+      <c r="D175" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A176" t="s">
+        <v>240</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A177" t="s">
+        <v>112</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C177" t="s">
+        <v>59</v>
+      </c>
+      <c r="D177" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A178" t="s">
+        <v>287</v>
+      </c>
+      <c r="B178" s="3" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A179" t="s">
+        <v>37</v>
+      </c>
+      <c r="B179" t="s">
+        <v>187</v>
+      </c>
+      <c r="C179" t="s">
+        <v>120</v>
+      </c>
+      <c r="D179" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A180" t="s">
+        <v>391</v>
+      </c>
+      <c r="B180" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A181" t="s">
+        <v>38</v>
+      </c>
+      <c r="B181" t="s">
+        <v>188</v>
+      </c>
+      <c r="C181" t="s">
+        <v>64</v>
+      </c>
+      <c r="D181" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A182" t="s">
+        <v>317</v>
+      </c>
+      <c r="B182" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A183" t="s">
+        <v>275</v>
+      </c>
+      <c r="B183" t="s">
+        <v>385</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D173">
-    <sortCondition ref="A139"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D183">
+    <sortCondition ref="A174"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
ch 6 end + start 7
</commit_message>
<xml_diff>
--- a/Index_of_terms.xlsx
+++ b/Index_of_terms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steffi\Documents\work\schmettow\GitHub\New_Stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB995B9A-B6F3-43A8-B1FE-110F94F625D0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCBD38E-FB1B-4860-AA5C-67BB5D03A1E6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="434">
   <si>
     <t>Term</t>
   </si>
@@ -1273,9 +1272,6 @@
     <t>Fixed effect</t>
   </si>
   <si>
-    <t>a fixed effect is a factor where levels are regarded so unsimilar, that the factor-level distribution can be practically considered infinite</t>
-  </si>
-  <si>
     <t>Psychometrics</t>
   </si>
   <si>
@@ -1301,6 +1297,54 @@
   </si>
   <si>
     <t>Between-subject design</t>
+  </si>
+  <si>
+    <t>Bayes theorem</t>
+  </si>
+  <si>
+    <t>Fundamental design research</t>
+  </si>
+  <si>
+    <t>Egan's assumption</t>
+  </si>
+  <si>
+    <t>Cross-classified random effects (CRE)</t>
+  </si>
+  <si>
+    <t>Interval-scaled test</t>
+  </si>
+  <si>
+    <t>Logistic regression</t>
+  </si>
+  <si>
+    <t>Law of smaller numbers</t>
+  </si>
+  <si>
+    <t>Pooling</t>
+  </si>
+  <si>
+    <t>A fixed effect is a factor where levels are regarded so unsimilar, that the factor-level distribution can be practically considered infinite.</t>
+  </si>
+  <si>
+    <t>Slope random effect</t>
+  </si>
+  <si>
+    <t>Within-entity design</t>
+  </si>
+  <si>
+    <t>Like within-subject design, but not necessarily with humans.</t>
+  </si>
+  <si>
+    <t>Link function</t>
+  </si>
+  <si>
+    <t>Pattern of randomness</t>
+  </si>
+  <si>
+    <t>Parametric model</t>
+  </si>
+  <si>
+    <t>Semiparametric model</t>
   </si>
 </sst>
 </file>
@@ -1631,10 +1675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D183"/>
+  <dimension ref="A1:D197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="B185" sqref="B185"/>
+    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
+      <selection activeCell="A198" sqref="A198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1747,1003 +1791,976 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>243</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>342</v>
-      </c>
-      <c r="C9" s="2">
-        <v>3</v>
+        <v>418</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>418</v>
+        <v>243</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="C10" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>74</v>
-      </c>
-      <c r="C11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" t="s">
-        <v>50</v>
+        <v>417</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>204</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>343</v>
+        <v>75</v>
       </c>
       <c r="C13" t="s">
-        <v>203</v>
+        <v>46</v>
       </c>
       <c r="D13" t="s">
-        <v>130</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>204</v>
       </c>
       <c r="B14" t="s">
-        <v>115</v>
+        <v>343</v>
       </c>
       <c r="C14" t="s">
-        <v>113</v>
+        <v>203</v>
       </c>
       <c r="D14" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>314</v>
+        <v>86</v>
       </c>
       <c r="B15" t="s">
-        <v>344</v>
+        <v>115</v>
       </c>
       <c r="C15" t="s">
-        <v>345</v>
+        <v>113</v>
+      </c>
+      <c r="D15" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>229</v>
+        <v>314</v>
       </c>
       <c r="B16" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C16" t="s">
-        <v>193</v>
-      </c>
-      <c r="D16" t="s">
-        <v>130</v>
+        <v>345</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>254</v>
+        <v>229</v>
       </c>
       <c r="B17" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C17" t="s">
-        <v>347</v>
+        <v>193</v>
+      </c>
+      <c r="D17" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>254</v>
       </c>
       <c r="B18" t="s">
-        <v>116</v>
+        <v>348</v>
       </c>
       <c r="C18" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" t="s">
-        <v>51</v>
+        <v>347</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D19" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>253</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="C20" t="s">
-        <v>117</v>
+        <v>53</v>
       </c>
       <c r="D20" t="s">
-        <v>118</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>110</v>
+        <v>253</v>
       </c>
       <c r="B21" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="C21" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D21" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>334</v>
+        <v>110</v>
       </c>
       <c r="B22" t="s">
-        <v>335</v>
+        <v>122</v>
+      </c>
+      <c r="C22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>334</v>
       </c>
       <c r="B23" t="s">
-        <v>158</v>
-      </c>
-      <c r="C23" t="s">
-        <v>55</v>
-      </c>
-      <c r="D23" t="s">
-        <v>56</v>
+        <v>335</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>307</v>
+        <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>308</v>
+        <v>158</v>
+      </c>
+      <c r="C24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>206</v>
+        <v>307</v>
       </c>
       <c r="B25" t="s">
-        <v>289</v>
-      </c>
-      <c r="C25" t="s">
-        <v>207</v>
+        <v>308</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="B26" t="s">
-        <v>349</v>
+        <v>289</v>
       </c>
       <c r="C26" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B27" t="s">
-        <v>350</v>
+        <v>349</v>
+      </c>
+      <c r="C27" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="B28" t="s">
-        <v>351</v>
-      </c>
-      <c r="C28" t="s">
-        <v>147</v>
+        <v>350</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>320</v>
+        <v>191</v>
       </c>
       <c r="B29" t="s">
-        <v>352</v>
+        <v>351</v>
+      </c>
+      <c r="C29" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>8</v>
+        <v>320</v>
       </c>
       <c r="B30" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30" s="2">
-        <v>4</v>
-      </c>
-      <c r="D30" t="s">
-        <v>52</v>
+        <v>352</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>264</v>
+        <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>353</v>
-      </c>
-      <c r="C31" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="C31" s="2">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>217</v>
-      </c>
+        <v>264</v>
+      </c>
+      <c r="B32" t="s">
+        <v>353</v>
+      </c>
+      <c r="C32" s="2"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>11</v>
-      </c>
-      <c r="B33" t="s">
-        <v>159</v>
-      </c>
-      <c r="C33" t="s">
-        <v>57</v>
-      </c>
-      <c r="D33" t="s">
-        <v>58</v>
+        <v>421</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>12</v>
-      </c>
-      <c r="B34" t="s">
-        <v>160</v>
-      </c>
-      <c r="C34" t="s">
-        <v>59</v>
-      </c>
-      <c r="D34" t="s">
-        <v>60</v>
+        <v>217</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>84</v>
+        <v>11</v>
       </c>
       <c r="B35" t="s">
-        <v>85</v>
+        <v>159</v>
       </c>
       <c r="C35" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D35" t="s">
-        <v>123</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>92</v>
+        <v>12</v>
       </c>
       <c r="B36" t="s">
-        <v>93</v>
+        <v>160</v>
       </c>
       <c r="C36" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="D36" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>290</v>
+        <v>84</v>
       </c>
       <c r="B37" t="s">
-        <v>400</v>
+        <v>85</v>
       </c>
       <c r="C37" t="s">
-        <v>207</v>
+        <v>64</v>
+      </c>
+      <c r="D37" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="B38" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="C38" t="s">
         <v>46</v>
       </c>
       <c r="D38" t="s">
-        <v>124</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>220</v>
+        <v>290</v>
       </c>
       <c r="B39" t="s">
-        <v>221</v>
-      </c>
-      <c r="C39" s="2">
-        <v>5</v>
+        <v>400</v>
+      </c>
+      <c r="C39" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>329</v>
+        <v>13</v>
       </c>
       <c r="B40" t="s">
-        <v>354</v>
-      </c>
-      <c r="C40" s="2"/>
+        <v>76</v>
+      </c>
+      <c r="C40" t="s">
+        <v>46</v>
+      </c>
+      <c r="D40" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>411</v>
+        <v>220</v>
+      </c>
+      <c r="B41" t="s">
+        <v>221</v>
+      </c>
+      <c r="C41" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>111</v>
+        <v>329</v>
       </c>
       <c r="B42" t="s">
-        <v>161</v>
-      </c>
-      <c r="C42" t="s">
-        <v>126</v>
-      </c>
-      <c r="D42" t="s">
-        <v>125</v>
-      </c>
+        <v>354</v>
+      </c>
+      <c r="C42" s="2"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>202</v>
-      </c>
-      <c r="B43" t="s">
-        <v>284</v>
-      </c>
-      <c r="C43" t="s">
-        <v>203</v>
+        <v>410</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>315</v>
+        <v>111</v>
       </c>
       <c r="B44" t="s">
-        <v>355</v>
+        <v>161</v>
+      </c>
+      <c r="C44" t="s">
+        <v>126</v>
+      </c>
+      <c r="D44" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>309</v>
+        <v>202</v>
       </c>
       <c r="B45" t="s">
-        <v>310</v>
+        <v>284</v>
+      </c>
+      <c r="C45" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>280</v>
+        <v>315</v>
       </c>
       <c r="B46" t="s">
-        <v>356</v>
-      </c>
-      <c r="C46" t="s">
-        <v>281</v>
+        <v>355</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>14</v>
-      </c>
-      <c r="B47" t="s">
-        <v>101</v>
-      </c>
-      <c r="C47" s="2">
-        <v>4</v>
-      </c>
-      <c r="D47" t="s">
-        <v>61</v>
+        <v>420</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>263</v>
+        <v>309</v>
       </c>
       <c r="B48" t="s">
-        <v>357</v>
-      </c>
-      <c r="C48" s="2"/>
+        <v>310</v>
+      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>279</v>
-      </c>
-      <c r="C49" s="2"/>
+        <v>280</v>
+      </c>
+      <c r="B49" t="s">
+        <v>356</v>
+      </c>
+      <c r="C49" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>258</v>
+        <v>14</v>
       </c>
       <c r="B50" t="s">
-        <v>358</v>
-      </c>
-      <c r="C50" t="s">
-        <v>257</v>
+        <v>101</v>
+      </c>
+      <c r="C50" s="2">
+        <v>4</v>
+      </c>
+      <c r="D50" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>312</v>
+        <v>263</v>
       </c>
       <c r="B51" t="s">
-        <v>359</v>
-      </c>
+        <v>357</v>
+      </c>
+      <c r="C51" s="2"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>236</v>
-      </c>
-      <c r="B52" t="s">
-        <v>237</v>
+        <v>279</v>
       </c>
       <c r="C52" s="2"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>103</v>
+        <v>258</v>
       </c>
       <c r="B53" t="s">
-        <v>102</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D53" t="s">
-        <v>128</v>
+        <v>358</v>
+      </c>
+      <c r="C53" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>15</v>
+        <v>312</v>
       </c>
       <c r="B54" t="s">
-        <v>162</v>
-      </c>
-      <c r="C54" t="s">
-        <v>46</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>62</v>
+        <v>359</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>283</v>
+        <v>236</v>
       </c>
       <c r="B55" t="s">
-        <v>360</v>
-      </c>
-      <c r="D55" s="2"/>
+        <v>237</v>
+      </c>
+      <c r="C55" s="2"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>361</v>
+        <v>103</v>
       </c>
       <c r="B56" t="s">
-        <v>362</v>
-      </c>
-      <c r="C56" t="s">
-        <v>211</v>
-      </c>
-      <c r="D56" s="2"/>
+        <v>102</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D56" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>408</v>
+        <v>15</v>
       </c>
       <c r="B57" t="s">
-        <v>409</v>
+        <v>162</v>
+      </c>
+      <c r="C57" t="s">
+        <v>46</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="B58" t="s">
-        <v>401</v>
+        <v>360</v>
       </c>
       <c r="D58" s="2"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>336</v>
-      </c>
+        <v>361</v>
+      </c>
+      <c r="B59" t="s">
+        <v>362</v>
+      </c>
+      <c r="C59" t="s">
+        <v>211</v>
+      </c>
+      <c r="D59" s="2"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>16</v>
+        <v>408</v>
       </c>
       <c r="B60" t="s">
-        <v>40</v>
-      </c>
-      <c r="C60" t="s">
-        <v>63</v>
-      </c>
-      <c r="D60" t="s">
-        <v>62</v>
+        <v>426</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>259</v>
+        <v>278</v>
       </c>
       <c r="B61" t="s">
-        <v>260</v>
-      </c>
+        <v>401</v>
+      </c>
+      <c r="D61" s="2"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>304</v>
+        <v>336</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>238</v>
+        <v>16</v>
       </c>
       <c r="B63" t="s">
-        <v>363</v>
+        <v>40</v>
+      </c>
+      <c r="C63" t="s">
+        <v>63</v>
+      </c>
+      <c r="D63" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>231</v>
-      </c>
-      <c r="B64" t="s">
-        <v>163</v>
-      </c>
-      <c r="C64" t="s">
-        <v>53</v>
-      </c>
-      <c r="D64" t="s">
-        <v>129</v>
+        <v>419</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>268</v>
+        <v>259</v>
+      </c>
+      <c r="B65" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>17</v>
-      </c>
-      <c r="B66" t="s">
-        <v>164</v>
-      </c>
-      <c r="C66" t="s">
-        <v>63</v>
-      </c>
-      <c r="D66" t="s">
-        <v>130</v>
+        <v>304</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="B67" t="s">
-        <v>252</v>
-      </c>
-      <c r="C67" t="s">
-        <v>249</v>
+        <v>363</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>218</v>
+        <v>231</v>
       </c>
       <c r="B68" t="s">
-        <v>364</v>
+        <v>163</v>
+      </c>
+      <c r="C68" t="s">
+        <v>53</v>
+      </c>
+      <c r="D68" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>402</v>
+        <v>268</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>96</v>
+        <v>17</v>
       </c>
       <c r="B70" t="s">
-        <v>97</v>
+        <v>164</v>
       </c>
       <c r="C70" t="s">
-        <v>131</v>
+        <v>63</v>
       </c>
       <c r="D70" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>219</v>
+        <v>251</v>
+      </c>
+      <c r="B71" t="s">
+        <v>252</v>
+      </c>
+      <c r="C71" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>18</v>
+        <v>218</v>
       </c>
       <c r="B72" t="s">
-        <v>165</v>
-      </c>
-      <c r="C72" t="s">
-        <v>64</v>
-      </c>
-      <c r="D72" t="s">
-        <v>57</v>
+        <v>364</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>108</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C73" t="s">
-        <v>133</v>
-      </c>
-      <c r="D73" t="s">
-        <v>134</v>
+        <v>402</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>250</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>365</v>
+        <v>96</v>
+      </c>
+      <c r="B74" t="s">
+        <v>97</v>
+      </c>
+      <c r="C74" t="s">
+        <v>131</v>
+      </c>
+      <c r="D74" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>19</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C75" t="s">
-        <v>46</v>
-      </c>
-      <c r="D75" t="s">
-        <v>65</v>
+        <v>219</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>285</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>296</v>
+        <v>18</v>
+      </c>
+      <c r="B76" t="s">
+        <v>165</v>
       </c>
       <c r="C76" t="s">
-        <v>211</v>
+        <v>64</v>
+      </c>
+      <c r="D76" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>332</v>
+        <v>108</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C77" t="s">
+        <v>133</v>
+      </c>
+      <c r="D77" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>239</v>
+        <v>250</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>94</v>
+        <v>19</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="C79" t="s">
-        <v>131</v>
+        <v>46</v>
       </c>
       <c r="D79" t="s">
-        <v>135</v>
+        <v>65</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>20</v>
+        <v>285</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>168</v>
+        <v>296</v>
       </c>
       <c r="C80" t="s">
-        <v>49</v>
-      </c>
-      <c r="D80" t="s">
-        <v>66</v>
+        <v>211</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>21</v>
-      </c>
-      <c r="B81" t="s">
-        <v>41</v>
-      </c>
-      <c r="C81" t="s">
-        <v>55</v>
-      </c>
-      <c r="D81" t="s">
-        <v>67</v>
+        <v>332</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>255</v>
-      </c>
-      <c r="C82" t="s">
-        <v>257</v>
+        <v>239</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>413</v>
+        <v>422</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>230</v>
-      </c>
-      <c r="B84" t="s">
-        <v>367</v>
-      </c>
-      <c r="C84" s="2">
-        <v>5</v>
+        <v>94</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C84" t="s">
+        <v>131</v>
+      </c>
+      <c r="D84" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>210</v>
+        <v>20</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C85" t="s">
+        <v>49</v>
+      </c>
+      <c r="D85" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>333</v>
-      </c>
-      <c r="B86" t="s">
-        <v>369</v>
+        <v>424</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>274</v>
+        <v>21</v>
       </c>
       <c r="B87" t="s">
-        <v>368</v>
+        <v>41</v>
       </c>
       <c r="C87" t="s">
-        <v>147</v>
+        <v>55</v>
+      </c>
+      <c r="D87" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>68</v>
-      </c>
-      <c r="B88" t="s">
-        <v>169</v>
+        <v>255</v>
       </c>
       <c r="C88" t="s">
-        <v>46</v>
-      </c>
-      <c r="D88" t="s">
-        <v>69</v>
+        <v>257</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>99</v>
-      </c>
-      <c r="B89" t="s">
-        <v>98</v>
-      </c>
-      <c r="C89" t="s">
-        <v>59</v>
-      </c>
-      <c r="D89" t="s">
-        <v>136</v>
+        <v>412</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>331</v>
+        <v>230</v>
       </c>
       <c r="B90" t="s">
-        <v>370</v>
+        <v>367</v>
+      </c>
+      <c r="C90" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>313</v>
-      </c>
-      <c r="B91" t="s">
-        <v>371</v>
+        <v>210</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>262</v>
-      </c>
-      <c r="C92" t="s">
-        <v>257</v>
+        <v>333</v>
+      </c>
+      <c r="B92" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>109</v>
+        <v>274</v>
       </c>
       <c r="B93" t="s">
-        <v>171</v>
+        <v>368</v>
       </c>
       <c r="C93" t="s">
-        <v>137</v>
-      </c>
-      <c r="D93" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>225</v>
+        <v>68</v>
       </c>
       <c r="B94" t="s">
-        <v>372</v>
+        <v>169</v>
+      </c>
+      <c r="C94" t="s">
+        <v>46</v>
+      </c>
+      <c r="D94" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>83</v>
-      </c>
-      <c r="B95" t="s">
-        <v>261</v>
-      </c>
-      <c r="C95" t="s">
-        <v>139</v>
-      </c>
-      <c r="D95" t="s">
-        <v>140</v>
+        <v>423</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>244</v>
+        <v>99</v>
       </c>
       <c r="B96" t="s">
-        <v>265</v>
+        <v>98</v>
       </c>
       <c r="C96" t="s">
-        <v>249</v>
+        <v>59</v>
+      </c>
+      <c r="D96" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>246</v>
+        <v>331</v>
       </c>
       <c r="B97" t="s">
-        <v>269</v>
-      </c>
-      <c r="C97" t="s">
-        <v>249</v>
+        <v>370</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>276</v>
+        <v>313</v>
       </c>
       <c r="B98" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>226</v>
-      </c>
-      <c r="B99" t="s">
-        <v>374</v>
+        <v>262</v>
+      </c>
+      <c r="C99" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>405</v>
+        <v>109</v>
+      </c>
+      <c r="B100" t="s">
+        <v>171</v>
+      </c>
+      <c r="C100" t="s">
+        <v>137</v>
+      </c>
+      <c r="D100" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>305</v>
+        <v>225</v>
       </c>
       <c r="B101" t="s">
-        <v>306</v>
+        <v>372</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>245</v>
+        <v>83</v>
       </c>
       <c r="B102" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C102" t="s">
-        <v>249</v>
+        <v>139</v>
+      </c>
+      <c r="D102" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>302</v>
+        <v>244</v>
       </c>
       <c r="B103" t="s">
-        <v>303</v>
+        <v>265</v>
       </c>
       <c r="C103" t="s">
-        <v>213</v>
+        <v>249</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B104" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="C104" t="s">
         <v>249</v>
@@ -2751,800 +2768,900 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>248</v>
-      </c>
-      <c r="C105" t="s">
-        <v>249</v>
+        <v>276</v>
+      </c>
+      <c r="B105" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>311</v>
+        <v>226</v>
       </c>
       <c r="B106" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>297</v>
-      </c>
-      <c r="B107" t="s">
-        <v>298</v>
+        <v>405</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>209</v>
+        <v>305</v>
       </c>
       <c r="B108" t="s">
-        <v>299</v>
+        <v>306</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>294</v>
+        <v>245</v>
       </c>
       <c r="B109" t="s">
-        <v>295</v>
+        <v>267</v>
       </c>
       <c r="C109" t="s">
-        <v>292</v>
+        <v>249</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>23</v>
+        <v>302</v>
       </c>
       <c r="B110" t="s">
-        <v>77</v>
+        <v>303</v>
       </c>
       <c r="C110" t="s">
-        <v>46</v>
-      </c>
-      <c r="D110" t="s">
-        <v>72</v>
+        <v>213</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>87</v>
+        <v>247</v>
       </c>
       <c r="B111" t="s">
-        <v>172</v>
+        <v>266</v>
       </c>
       <c r="C111" t="s">
-        <v>113</v>
-      </c>
-      <c r="D111" t="s">
-        <v>130</v>
+        <v>249</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>407</v>
+        <v>248</v>
+      </c>
+      <c r="C112" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>330</v>
+        <v>311</v>
+      </c>
+      <c r="B113" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>337</v>
+        <v>297</v>
       </c>
       <c r="B114" t="s">
-        <v>376</v>
+        <v>298</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B115" t="s">
-        <v>271</v>
-      </c>
-      <c r="C115" t="s">
-        <v>213</v>
+        <v>299</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>24</v>
+        <v>294</v>
       </c>
       <c r="B116" t="s">
-        <v>173</v>
+        <v>295</v>
       </c>
       <c r="C116" t="s">
-        <v>46</v>
-      </c>
-      <c r="D116" t="s">
-        <v>73</v>
+        <v>292</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B117" t="s">
-        <v>174</v>
+        <v>77</v>
       </c>
       <c r="C117" t="s">
         <v>46</v>
       </c>
       <c r="D117" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>26</v>
-      </c>
-      <c r="B118" s="3" t="s">
-        <v>175</v>
+        <v>87</v>
+      </c>
+      <c r="B118" t="s">
+        <v>172</v>
       </c>
       <c r="C118" t="s">
-        <v>49</v>
+        <v>113</v>
       </c>
       <c r="D118" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>88</v>
-      </c>
-      <c r="B119" t="s">
-        <v>89</v>
-      </c>
-      <c r="C119" t="s">
-        <v>131</v>
-      </c>
-      <c r="D119" t="s">
-        <v>130</v>
+        <v>407</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>27</v>
-      </c>
-      <c r="B120" t="s">
-        <v>100</v>
-      </c>
-      <c r="C120" t="s">
-        <v>57</v>
-      </c>
-      <c r="D120" t="s">
-        <v>142</v>
+        <v>330</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>28</v>
+        <v>337</v>
       </c>
       <c r="B121" t="s">
-        <v>42</v>
-      </c>
-      <c r="C121" t="s">
-        <v>55</v>
-      </c>
-      <c r="D121" t="s">
-        <v>143</v>
+        <v>376</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>316</v>
+        <v>212</v>
       </c>
       <c r="B122" t="s">
-        <v>377</v>
+        <v>271</v>
+      </c>
+      <c r="C122" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="B123" t="s">
-        <v>81</v>
+        <v>173</v>
       </c>
       <c r="C123" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D123" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>272</v>
+        <v>25</v>
+      </c>
+      <c r="B124" t="s">
+        <v>174</v>
       </c>
       <c r="C124" t="s">
-        <v>139</v>
+        <v>46</v>
+      </c>
+      <c r="D124" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>90</v>
-      </c>
-      <c r="B125" t="s">
-        <v>91</v>
+        <v>26</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="C125" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D125" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>277</v>
+        <v>88</v>
       </c>
       <c r="B126" t="s">
-        <v>378</v>
+        <v>89</v>
+      </c>
+      <c r="C126" t="s">
+        <v>131</v>
+      </c>
+      <c r="D126" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B127" t="s">
-        <v>176</v>
+        <v>100</v>
       </c>
       <c r="C127" t="s">
-        <v>127</v>
+        <v>57</v>
       </c>
       <c r="D127" t="s">
-        <v>62</v>
+        <v>142</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>82</v>
-      </c>
-      <c r="B128" s="3" t="s">
-        <v>177</v>
+        <v>28</v>
+      </c>
+      <c r="B128" t="s">
+        <v>42</v>
       </c>
       <c r="C128" t="s">
-        <v>145</v>
+        <v>55</v>
       </c>
       <c r="D128" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>30</v>
+        <v>316</v>
       </c>
       <c r="B129" t="s">
-        <v>78</v>
-      </c>
-      <c r="C129" t="s">
-        <v>49</v>
-      </c>
-      <c r="D129" t="s">
-        <v>130</v>
+        <v>377</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>232</v>
+        <v>80</v>
       </c>
       <c r="B130" t="s">
-        <v>379</v>
+        <v>81</v>
+      </c>
+      <c r="C130" t="s">
+        <v>49</v>
+      </c>
+      <c r="D130" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>319</v>
-      </c>
-      <c r="B131" t="s">
-        <v>380</v>
+        <v>272</v>
+      </c>
+      <c r="C131" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>200</v>
+        <v>90</v>
+      </c>
+      <c r="B132" t="s">
+        <v>91</v>
+      </c>
+      <c r="C132" t="s">
+        <v>46</v>
+      </c>
+      <c r="D132" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>222</v>
+        <v>277</v>
+      </c>
+      <c r="B133" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>282</v>
+        <v>29</v>
+      </c>
+      <c r="B134" t="s">
+        <v>176</v>
+      </c>
+      <c r="C134" t="s">
+        <v>127</v>
+      </c>
+      <c r="D134" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>223</v>
+        <v>82</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C135" t="s">
+        <v>145</v>
+      </c>
+      <c r="D135" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>233</v>
+        <v>30</v>
       </c>
       <c r="B136" t="s">
-        <v>234</v>
+        <v>78</v>
+      </c>
+      <c r="C136" t="s">
+        <v>49</v>
+      </c>
+      <c r="D136" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>192</v>
-      </c>
-      <c r="B137" t="s">
-        <v>381</v>
-      </c>
-      <c r="C137" t="s">
-        <v>193</v>
+        <v>425</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>322</v>
+        <v>232</v>
       </c>
       <c r="B138" t="s">
-        <v>323</v>
+        <v>379</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>273</v>
+        <v>319</v>
+      </c>
+      <c r="B139" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>321</v>
-      </c>
-      <c r="B140" t="s">
-        <v>382</v>
+        <v>200</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>410</v>
+        <v>222</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>270</v>
-      </c>
-      <c r="B142" t="s">
-        <v>383</v>
+        <v>282</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>215</v>
-      </c>
-      <c r="C143" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>214</v>
+        <v>233</v>
       </c>
       <c r="B144" t="s">
-        <v>384</v>
-      </c>
-      <c r="C144" t="s">
-        <v>213</v>
+        <v>234</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>31</v>
+        <v>192</v>
       </c>
       <c r="B145" t="s">
-        <v>43</v>
-      </c>
-      <c r="C145" s="2">
-        <v>4</v>
-      </c>
-      <c r="D145" t="s">
-        <v>62</v>
+        <v>381</v>
+      </c>
+      <c r="C145" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>32</v>
+        <v>322</v>
       </c>
       <c r="B146" t="s">
-        <v>44</v>
-      </c>
-      <c r="C146" t="s">
-        <v>55</v>
-      </c>
-      <c r="D146" t="s">
-        <v>137</v>
+        <v>323</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>406</v>
-      </c>
-      <c r="B147" t="s">
-        <v>416</v>
+        <v>273</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>403</v>
+        <v>321</v>
       </c>
       <c r="B148" t="s">
-        <v>404</v>
+        <v>382</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>256</v>
+        <v>270</v>
       </c>
       <c r="B150" t="s">
-        <v>399</v>
-      </c>
-      <c r="C150" t="s">
-        <v>257</v>
+        <v>383</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>195</v>
-      </c>
-      <c r="B151" t="s">
-        <v>398</v>
-      </c>
-      <c r="C151" s="2" t="s">
-        <v>139</v>
+        <v>215</v>
+      </c>
+      <c r="C151" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>324</v>
+        <v>214</v>
       </c>
       <c r="B152" t="s">
-        <v>397</v>
+        <v>384</v>
+      </c>
+      <c r="C152" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>415</v>
+        <v>31</v>
+      </c>
+      <c r="B153" t="s">
+        <v>43</v>
+      </c>
+      <c r="C153" s="2">
+        <v>4</v>
+      </c>
+      <c r="D153" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>286</v>
+        <v>32</v>
       </c>
       <c r="B154" t="s">
-        <v>288</v>
-      </c>
-      <c r="C154" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="C154" t="s">
+        <v>55</v>
+      </c>
+      <c r="D154" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>105</v>
+        <v>406</v>
       </c>
       <c r="B155" t="s">
-        <v>178</v>
-      </c>
-      <c r="C155" t="s">
-        <v>147</v>
-      </c>
-      <c r="D155" t="s">
-        <v>62</v>
+        <v>415</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>106</v>
+        <v>403</v>
       </c>
       <c r="B156" t="s">
-        <v>179</v>
-      </c>
-      <c r="C156" t="s">
-        <v>148</v>
-      </c>
-      <c r="D156" t="s">
-        <v>149</v>
+        <v>404</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>107</v>
-      </c>
-      <c r="B157" t="s">
-        <v>180</v>
-      </c>
-      <c r="C157" t="s">
-        <v>148</v>
-      </c>
-      <c r="D157" t="s">
-        <v>150</v>
+        <v>416</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>318</v>
+        <v>256</v>
       </c>
       <c r="B158" t="s">
-        <v>396</v>
+        <v>399</v>
+      </c>
+      <c r="C158" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>235</v>
+        <v>195</v>
       </c>
       <c r="B159" t="s">
-        <v>395</v>
+        <v>398</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>181</v>
+        <v>324</v>
       </c>
       <c r="B160" t="s">
-        <v>182</v>
-      </c>
-      <c r="C160" t="s">
-        <v>151</v>
-      </c>
-      <c r="D160" t="s">
-        <v>152</v>
+        <v>397</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>328</v>
-      </c>
-      <c r="B161" t="s">
-        <v>393</v>
+        <v>414</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>33</v>
+        <v>286</v>
       </c>
       <c r="B162" t="s">
-        <v>183</v>
-      </c>
-      <c r="C162" t="s">
-        <v>49</v>
-      </c>
-      <c r="D162" t="s">
-        <v>153</v>
-      </c>
+        <v>288</v>
+      </c>
+      <c r="C162" s="2"/>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>194</v>
+        <v>105</v>
       </c>
       <c r="B163" t="s">
-        <v>394</v>
+        <v>178</v>
       </c>
       <c r="C163" t="s">
-        <v>193</v>
+        <v>147</v>
+      </c>
+      <c r="D163" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>412</v>
+        <v>106</v>
+      </c>
+      <c r="B164" t="s">
+        <v>179</v>
+      </c>
+      <c r="C164" t="s">
+        <v>148</v>
+      </c>
+      <c r="D164" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>189</v>
+        <v>107</v>
       </c>
       <c r="B165" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="C165" t="s">
-        <v>147</v>
+        <v>148</v>
+      </c>
+      <c r="D165" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>196</v>
+        <v>318</v>
       </c>
       <c r="B166" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
       <c r="B167" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>34</v>
+        <v>181</v>
       </c>
       <c r="B168" t="s">
-        <v>79</v>
-      </c>
-      <c r="C168" s="2">
-        <v>1</v>
+        <v>182</v>
+      </c>
+      <c r="C168" t="s">
+        <v>151</v>
       </c>
       <c r="D168" t="s">
-        <v>136</v>
+        <v>152</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>35</v>
-      </c>
-      <c r="B169" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C169" s="2">
-        <v>4</v>
-      </c>
-      <c r="D169" t="s">
-        <v>154</v>
+        <v>328</v>
+      </c>
+      <c r="B169" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>325</v>
-      </c>
-      <c r="B170" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="C170" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="B170" t="s">
+        <v>183</v>
+      </c>
+      <c r="C170" t="s">
+        <v>49</v>
+      </c>
+      <c r="D170" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>22</v>
-      </c>
-      <c r="B171" s="3" t="s">
-        <v>170</v>
+        <v>194</v>
+      </c>
+      <c r="B171" t="s">
+        <v>394</v>
       </c>
       <c r="C171" t="s">
-        <v>70</v>
-      </c>
-      <c r="D171" t="s">
-        <v>71</v>
+        <v>193</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>208</v>
-      </c>
-      <c r="B173" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="C173" s="2" t="s">
-        <v>207</v>
+        <v>427</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>36</v>
+        <v>189</v>
       </c>
       <c r="B174" t="s">
-        <v>45</v>
-      </c>
-      <c r="C174" s="2">
-        <v>4</v>
-      </c>
-      <c r="D174" t="s">
-        <v>155</v>
+        <v>190</v>
+      </c>
+      <c r="C174" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>95</v>
-      </c>
-      <c r="B175" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="C175" t="s">
-        <v>46</v>
-      </c>
-      <c r="D175" t="s">
-        <v>62</v>
+        <v>196</v>
+      </c>
+      <c r="B175" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>240</v>
-      </c>
-      <c r="B176" s="3" t="s">
-        <v>241</v>
+        <v>224</v>
+      </c>
+      <c r="B176" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>112</v>
-      </c>
-      <c r="B177" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="C177" t="s">
-        <v>59</v>
+        <v>34</v>
+      </c>
+      <c r="B177" t="s">
+        <v>79</v>
+      </c>
+      <c r="C177" s="2">
+        <v>1</v>
       </c>
       <c r="D177" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>287</v>
+        <v>35</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>387</v>
+        <v>184</v>
+      </c>
+      <c r="C178" s="2">
+        <v>4</v>
+      </c>
+      <c r="D178" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>37</v>
-      </c>
-      <c r="B179" t="s">
-        <v>187</v>
-      </c>
-      <c r="C179" t="s">
-        <v>120</v>
-      </c>
-      <c r="D179" t="s">
-        <v>62</v>
-      </c>
+        <v>325</v>
+      </c>
+      <c r="B179" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C179" s="2"/>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>391</v>
-      </c>
-      <c r="B180" t="s">
-        <v>392</v>
+        <v>22</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C180" t="s">
+        <v>70</v>
+      </c>
+      <c r="D180" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>38</v>
-      </c>
-      <c r="B181" t="s">
-        <v>188</v>
-      </c>
-      <c r="C181" t="s">
-        <v>64</v>
-      </c>
-      <c r="D181" t="s">
-        <v>157</v>
+        <v>413</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>317</v>
-      </c>
-      <c r="B182" t="s">
-        <v>386</v>
+        <v>208</v>
+      </c>
+      <c r="B182" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
+        <v>36</v>
+      </c>
+      <c r="B183" t="s">
+        <v>45</v>
+      </c>
+      <c r="C183" s="2">
+        <v>4</v>
+      </c>
+      <c r="D183" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A184" t="s">
+        <v>95</v>
+      </c>
+      <c r="B184" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C184" t="s">
+        <v>46</v>
+      </c>
+      <c r="D184" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A185" t="s">
+        <v>240</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A186" t="s">
+        <v>112</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C186" t="s">
+        <v>59</v>
+      </c>
+      <c r="D186" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A187" t="s">
+        <v>287</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A188" t="s">
+        <v>37</v>
+      </c>
+      <c r="B188" t="s">
+        <v>187</v>
+      </c>
+      <c r="C188" t="s">
+        <v>120</v>
+      </c>
+      <c r="D188" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A189" t="s">
+        <v>391</v>
+      </c>
+      <c r="B189" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A190" t="s">
+        <v>38</v>
+      </c>
+      <c r="B190" t="s">
+        <v>188</v>
+      </c>
+      <c r="C190" t="s">
+        <v>64</v>
+      </c>
+      <c r="D190" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A191" t="s">
+        <v>428</v>
+      </c>
+      <c r="B191" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A192" t="s">
+        <v>317</v>
+      </c>
+      <c r="B192" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A193" t="s">
         <v>275</v>
       </c>
-      <c r="B183" t="s">
+      <c r="B193" t="s">
         <v>385</v>
       </c>
     </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A194" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A195" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A196" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A197" t="s">
+        <v>433</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D183">
-    <sortCondition ref="A174"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D193">
+    <sortCondition ref="A193"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
ch7 comments + spelling
</commit_message>
<xml_diff>
--- a/Index_of_terms.xlsx
+++ b/Index_of_terms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steffi\Documents\work\schmettow\GitHub\New_Stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C367DAD0-3556-4D34-A763-1FF693AB3CB9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E8F442-12AB-493A-A353-804B093369AB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="475">
   <si>
     <t>Term</t>
   </si>
@@ -1448,6 +1447,27 @@
   </si>
   <si>
     <t>Distributional model</t>
+  </si>
+  <si>
+    <t>Censoring (lower/higher bound, interval)</t>
+  </si>
+  <si>
+    <t>Hedonistic values</t>
+  </si>
+  <si>
+    <t>Anchoring</t>
+  </si>
+  <si>
+    <t>Binning</t>
+  </si>
+  <si>
+    <t>Beta regression</t>
+  </si>
+  <si>
+    <t>cratio</t>
+  </si>
+  <si>
+    <t>Scale parameter</t>
   </si>
 </sst>
 </file>
@@ -1777,10 +1797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D225"/>
+  <dimension ref="A1:D232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="A200" workbookViewId="0">
+      <selection activeCell="B207" sqref="A207:XFD207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1843,1199 +1863,1183 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>201</v>
-      </c>
-      <c r="B5" t="s">
-        <v>340</v>
-      </c>
-      <c r="C5" t="s">
-        <v>117</v>
-      </c>
-      <c r="D5" t="s">
-        <v>228</v>
+        <v>470</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>201</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>340</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>117</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>242</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>341</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>46</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>300</v>
+        <v>242</v>
       </c>
       <c r="B8" t="s">
-        <v>301</v>
+        <v>341</v>
       </c>
       <c r="C8" t="s">
-        <v>213</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>418</v>
+        <v>300</v>
+      </c>
+      <c r="B9" t="s">
+        <v>301</v>
+      </c>
+      <c r="C9" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>243</v>
-      </c>
-      <c r="B10" t="s">
-        <v>342</v>
-      </c>
-      <c r="C10" s="2">
-        <v>3</v>
+        <v>418</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>447</v>
-      </c>
-      <c r="C11" s="2"/>
+        <v>243</v>
+      </c>
+      <c r="B11" t="s">
+        <v>342</v>
+      </c>
+      <c r="C11" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>417</v>
-      </c>
+        <v>447</v>
+      </c>
+      <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>458</v>
-      </c>
+        <v>472</v>
+      </c>
+      <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>443</v>
+        <v>417</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" t="s">
-        <v>50</v>
+        <v>458</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" t="s">
-        <v>49</v>
+        <v>443</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>204</v>
-      </c>
-      <c r="B18" t="s">
-        <v>343</v>
-      </c>
-      <c r="C18" t="s">
-        <v>203</v>
-      </c>
-      <c r="D18" t="s">
-        <v>130</v>
+        <v>459</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>457</v>
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>448</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>449</v>
+        <v>75</v>
+      </c>
+      <c r="C20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>434</v>
+        <v>204</v>
+      </c>
+      <c r="B21" t="s">
+        <v>343</v>
+      </c>
+      <c r="C21" t="s">
+        <v>203</v>
+      </c>
+      <c r="D21" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>86</v>
-      </c>
-      <c r="B22" t="s">
-        <v>115</v>
-      </c>
-      <c r="C22" t="s">
-        <v>113</v>
-      </c>
-      <c r="D22" t="s">
-        <v>114</v>
+        <v>457</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>314</v>
+        <v>448</v>
       </c>
       <c r="B23" t="s">
-        <v>344</v>
-      </c>
-      <c r="C23" t="s">
-        <v>345</v>
+        <v>449</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>461</v>
+        <v>434</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>229</v>
+        <v>86</v>
       </c>
       <c r="B25" t="s">
-        <v>346</v>
+        <v>115</v>
       </c>
       <c r="C25" t="s">
-        <v>193</v>
+        <v>113</v>
       </c>
       <c r="D25" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>254</v>
+        <v>314</v>
       </c>
       <c r="B26" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" t="s">
-        <v>116</v>
-      </c>
-      <c r="C27" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" t="s">
-        <v>51</v>
+        <v>461</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>453</v>
+        <v>468</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>9</v>
+        <v>229</v>
       </c>
       <c r="B29" t="s">
-        <v>119</v>
+        <v>346</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
+        <v>193</v>
       </c>
       <c r="D29" t="s">
-        <v>54</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B30" t="s">
-        <v>104</v>
+        <v>348</v>
       </c>
       <c r="C30" t="s">
-        <v>117</v>
-      </c>
-      <c r="D30" t="s">
-        <v>118</v>
+        <v>347</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>110</v>
+        <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C31" t="s">
-        <v>120</v>
+        <v>46</v>
       </c>
       <c r="D31" t="s">
-        <v>121</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>334</v>
-      </c>
-      <c r="B32" t="s">
-        <v>335</v>
+        <v>453</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B33" t="s">
-        <v>158</v>
+        <v>119</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D33" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>436</v>
+        <v>253</v>
+      </c>
+      <c r="B34" t="s">
+        <v>104</v>
+      </c>
+      <c r="C34" t="s">
+        <v>117</v>
+      </c>
+      <c r="D34" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>307</v>
+        <v>110</v>
       </c>
       <c r="B35" t="s">
-        <v>308</v>
+        <v>122</v>
+      </c>
+      <c r="C35" t="s">
+        <v>120</v>
+      </c>
+      <c r="D35" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>206</v>
+        <v>334</v>
       </c>
       <c r="B36" t="s">
-        <v>289</v>
-      </c>
-      <c r="C36" t="s">
-        <v>207</v>
+        <v>335</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>197</v>
+        <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>349</v>
+        <v>158</v>
       </c>
       <c r="C37" t="s">
-        <v>198</v>
+        <v>55</v>
+      </c>
+      <c r="D37" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>199</v>
-      </c>
-      <c r="B38" t="s">
-        <v>350</v>
+        <v>436</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>191</v>
+        <v>307</v>
       </c>
       <c r="B39" t="s">
-        <v>351</v>
-      </c>
-      <c r="C39" t="s">
-        <v>147</v>
+        <v>308</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>320</v>
+        <v>206</v>
       </c>
       <c r="B40" t="s">
-        <v>352</v>
+        <v>289</v>
+      </c>
+      <c r="C40" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>8</v>
+        <v>197</v>
       </c>
       <c r="B41" t="s">
-        <v>39</v>
-      </c>
-      <c r="C41" s="2">
-        <v>4</v>
-      </c>
-      <c r="D41" t="s">
-        <v>52</v>
+        <v>349</v>
+      </c>
+      <c r="C41" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>264</v>
+        <v>199</v>
       </c>
       <c r="B42" t="s">
-        <v>353</v>
-      </c>
-      <c r="C42" s="2"/>
+        <v>350</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>421</v>
+        <v>191</v>
+      </c>
+      <c r="B43" t="s">
+        <v>351</v>
+      </c>
+      <c r="C43" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>217</v>
+        <v>320</v>
+      </c>
+      <c r="B44" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B45" t="s">
-        <v>159</v>
-      </c>
-      <c r="C45" t="s">
-        <v>57</v>
+        <v>39</v>
+      </c>
+      <c r="C45" s="2">
+        <v>4</v>
       </c>
       <c r="D45" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>12</v>
-      </c>
-      <c r="B46" t="s">
-        <v>160</v>
-      </c>
-      <c r="C46" t="s">
-        <v>59</v>
-      </c>
-      <c r="D46" t="s">
-        <v>60</v>
-      </c>
+        <v>473</v>
+      </c>
+      <c r="C46" s="2"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>84</v>
+        <v>264</v>
       </c>
       <c r="B47" t="s">
-        <v>85</v>
-      </c>
-      <c r="C47" t="s">
-        <v>64</v>
-      </c>
-      <c r="D47" t="s">
-        <v>123</v>
-      </c>
+        <v>353</v>
+      </c>
+      <c r="C47" s="2"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>92</v>
-      </c>
-      <c r="B48" t="s">
-        <v>93</v>
-      </c>
-      <c r="C48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D48" t="s">
-        <v>62</v>
+        <v>421</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>290</v>
-      </c>
-      <c r="B49" t="s">
-        <v>400</v>
-      </c>
-      <c r="C49" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B50" t="s">
-        <v>76</v>
+        <v>159</v>
       </c>
       <c r="C50" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="D50" t="s">
-        <v>124</v>
+        <v>58</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>220</v>
+        <v>12</v>
       </c>
       <c r="B51" t="s">
-        <v>221</v>
-      </c>
-      <c r="C51" s="2">
-        <v>5</v>
+        <v>160</v>
+      </c>
+      <c r="C51" t="s">
+        <v>59</v>
+      </c>
+      <c r="D51" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>329</v>
+        <v>84</v>
       </c>
       <c r="B52" t="s">
-        <v>354</v>
-      </c>
-      <c r="C52" s="2"/>
+        <v>85</v>
+      </c>
+      <c r="C52" t="s">
+        <v>64</v>
+      </c>
+      <c r="D52" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>410</v>
+        <v>92</v>
+      </c>
+      <c r="B53" t="s">
+        <v>93</v>
+      </c>
+      <c r="C53" t="s">
+        <v>46</v>
+      </c>
+      <c r="D53" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>467</v>
+        <v>290</v>
+      </c>
+      <c r="B54" t="s">
+        <v>400</v>
+      </c>
+      <c r="C54" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>111</v>
+        <v>13</v>
       </c>
       <c r="B55" t="s">
-        <v>161</v>
+        <v>76</v>
       </c>
       <c r="C55" t="s">
-        <v>126</v>
+        <v>46</v>
       </c>
       <c r="D55" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="B56" t="s">
-        <v>284</v>
-      </c>
-      <c r="C56" t="s">
-        <v>203</v>
+        <v>221</v>
+      </c>
+      <c r="C56" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="B57" t="s">
-        <v>355</v>
-      </c>
+        <v>354</v>
+      </c>
+      <c r="C57" s="2"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>309</v>
-      </c>
-      <c r="B59" t="s">
-        <v>310</v>
+        <v>467</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>280</v>
+        <v>111</v>
       </c>
       <c r="B60" t="s">
-        <v>356</v>
+        <v>161</v>
       </c>
       <c r="C60" t="s">
-        <v>281</v>
+        <v>126</v>
+      </c>
+      <c r="D60" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>14</v>
+        <v>202</v>
       </c>
       <c r="B61" t="s">
-        <v>101</v>
-      </c>
-      <c r="C61" s="2">
-        <v>4</v>
-      </c>
-      <c r="D61" t="s">
-        <v>61</v>
+        <v>284</v>
+      </c>
+      <c r="C61" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>263</v>
+        <v>315</v>
       </c>
       <c r="B62" t="s">
-        <v>357</v>
-      </c>
-      <c r="C62" s="2"/>
+        <v>355</v>
+      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>279</v>
-      </c>
-      <c r="C63" s="2"/>
+        <v>420</v>
+      </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>444</v>
-      </c>
-      <c r="C64" s="2"/>
+        <v>309</v>
+      </c>
+      <c r="B64" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="B65" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C65" t="s">
-        <v>257</v>
+        <v>281</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>312</v>
+        <v>14</v>
       </c>
       <c r="B66" t="s">
-        <v>359</v>
+        <v>101</v>
+      </c>
+      <c r="C66" s="2">
+        <v>4</v>
+      </c>
+      <c r="D66" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>236</v>
+        <v>263</v>
       </c>
       <c r="B67" t="s">
-        <v>237</v>
+        <v>357</v>
       </c>
       <c r="C67" s="2"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>103</v>
-      </c>
-      <c r="B68" t="s">
-        <v>102</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D68" t="s">
-        <v>128</v>
-      </c>
+        <v>279</v>
+      </c>
+      <c r="C68" s="2"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>15</v>
-      </c>
-      <c r="B69" t="s">
-        <v>162</v>
-      </c>
-      <c r="C69" t="s">
-        <v>46</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>62</v>
-      </c>
+        <v>444</v>
+      </c>
+      <c r="C69" s="2"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>283</v>
+        <v>258</v>
       </c>
       <c r="B70" t="s">
-        <v>360</v>
-      </c>
-      <c r="D70" s="2"/>
+        <v>358</v>
+      </c>
+      <c r="C70" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>361</v>
+        <v>312</v>
       </c>
       <c r="B71" t="s">
-        <v>362</v>
-      </c>
-      <c r="C71" t="s">
-        <v>211</v>
-      </c>
-      <c r="D71" s="2"/>
+        <v>359</v>
+      </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>408</v>
+        <v>236</v>
       </c>
       <c r="B72" t="s">
-        <v>426</v>
-      </c>
+        <v>237</v>
+      </c>
+      <c r="C72" s="2"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>454</v>
-      </c>
-      <c r="D73" s="2"/>
+        <v>103</v>
+      </c>
+      <c r="B73" t="s">
+        <v>102</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D73" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>278</v>
+        <v>15</v>
       </c>
       <c r="B74" t="s">
-        <v>401</v>
-      </c>
-      <c r="D74" s="2"/>
+        <v>162</v>
+      </c>
+      <c r="C74" t="s">
+        <v>46</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>336</v>
-      </c>
+        <v>283</v>
+      </c>
+      <c r="B75" t="s">
+        <v>360</v>
+      </c>
+      <c r="D75" s="2"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>16</v>
+        <v>361</v>
       </c>
       <c r="B76" t="s">
-        <v>40</v>
+        <v>362</v>
       </c>
       <c r="C76" t="s">
-        <v>63</v>
-      </c>
-      <c r="D76" t="s">
-        <v>62</v>
-      </c>
+        <v>211</v>
+      </c>
+      <c r="D76" s="2"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>419</v>
+        <v>408</v>
+      </c>
+      <c r="B77" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>445</v>
-      </c>
+        <v>454</v>
+      </c>
+      <c r="D78" s="2"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>259</v>
+        <v>278</v>
       </c>
       <c r="B79" t="s">
-        <v>260</v>
-      </c>
+        <v>401</v>
+      </c>
+      <c r="D79" s="2"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>439</v>
+        <v>336</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>304</v>
+        <v>16</v>
+      </c>
+      <c r="B81" t="s">
+        <v>40</v>
+      </c>
+      <c r="C81" t="s">
+        <v>63</v>
+      </c>
+      <c r="D81" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>238</v>
-      </c>
-      <c r="B82" t="s">
-        <v>363</v>
+        <v>419</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>231</v>
-      </c>
-      <c r="B83" t="s">
-        <v>163</v>
-      </c>
-      <c r="C83" t="s">
-        <v>53</v>
-      </c>
-      <c r="D83" t="s">
-        <v>129</v>
+        <v>445</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>268</v>
+        <v>259</v>
+      </c>
+      <c r="B84" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>17</v>
-      </c>
-      <c r="B85" t="s">
-        <v>164</v>
-      </c>
-      <c r="C85" t="s">
-        <v>63</v>
-      </c>
-      <c r="D85" t="s">
-        <v>130</v>
+        <v>439</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>251</v>
-      </c>
-      <c r="B86" t="s">
-        <v>252</v>
-      </c>
-      <c r="C86" t="s">
-        <v>249</v>
+        <v>304</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>218</v>
+        <v>238</v>
       </c>
       <c r="B87" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>402</v>
+        <v>231</v>
+      </c>
+      <c r="B88" t="s">
+        <v>163</v>
+      </c>
+      <c r="C88" t="s">
+        <v>53</v>
+      </c>
+      <c r="D88" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>96</v>
-      </c>
-      <c r="B89" t="s">
-        <v>97</v>
-      </c>
-      <c r="C89" t="s">
-        <v>131</v>
-      </c>
-      <c r="D89" t="s">
-        <v>132</v>
+        <v>469</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>219</v>
+        <v>268</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B91" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C91" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D91" t="s">
-        <v>57</v>
+        <v>130</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>108</v>
+        <v>251</v>
       </c>
       <c r="B92" t="s">
-        <v>166</v>
+        <v>252</v>
       </c>
       <c r="C92" t="s">
-        <v>133</v>
-      </c>
-      <c r="D92" t="s">
-        <v>134</v>
+        <v>249</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>250</v>
+        <v>218</v>
       </c>
       <c r="B93" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>19</v>
-      </c>
-      <c r="B94" t="s">
-        <v>167</v>
-      </c>
-      <c r="C94" t="s">
-        <v>46</v>
-      </c>
-      <c r="D94" t="s">
-        <v>65</v>
+        <v>402</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>285</v>
+        <v>96</v>
       </c>
       <c r="B95" t="s">
-        <v>296</v>
+        <v>97</v>
       </c>
       <c r="C95" t="s">
-        <v>211</v>
+        <v>131</v>
+      </c>
+      <c r="D95" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>332</v>
+        <v>219</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>239</v>
+        <v>18</v>
       </c>
       <c r="B97" t="s">
-        <v>366</v>
+        <v>165</v>
+      </c>
+      <c r="C97" t="s">
+        <v>64</v>
+      </c>
+      <c r="D97" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>422</v>
+        <v>108</v>
+      </c>
+      <c r="B98" t="s">
+        <v>166</v>
+      </c>
+      <c r="C98" t="s">
+        <v>133</v>
+      </c>
+      <c r="D98" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>450</v>
+        <v>250</v>
+      </c>
+      <c r="B99" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>94</v>
+        <v>19</v>
       </c>
       <c r="B100" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="C100" t="s">
-        <v>131</v>
+        <v>46</v>
       </c>
       <c r="D100" t="s">
-        <v>135</v>
+        <v>65</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>20</v>
+        <v>285</v>
       </c>
       <c r="B101" t="s">
-        <v>168</v>
+        <v>296</v>
       </c>
       <c r="C101" t="s">
-        <v>49</v>
-      </c>
-      <c r="D101" t="s">
-        <v>66</v>
+        <v>211</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>424</v>
+        <v>332</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>455</v>
-      </c>
-      <c r="C103" t="s">
-        <v>456</v>
+        <v>239</v>
+      </c>
+      <c r="B103" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>21</v>
-      </c>
-      <c r="B104" t="s">
-        <v>41</v>
-      </c>
-      <c r="C104" t="s">
-        <v>55</v>
-      </c>
-      <c r="D104" t="s">
-        <v>67</v>
+        <v>422</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>435</v>
+        <v>450</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>255</v>
+        <v>94</v>
+      </c>
+      <c r="B106" t="s">
+        <v>185</v>
       </c>
       <c r="C106" t="s">
-        <v>257</v>
+        <v>131</v>
+      </c>
+      <c r="D106" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>412</v>
+        <v>20</v>
+      </c>
+      <c r="B107" t="s">
+        <v>168</v>
+      </c>
+      <c r="C107" t="s">
+        <v>49</v>
+      </c>
+      <c r="D107" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>230</v>
-      </c>
-      <c r="B108" t="s">
-        <v>367</v>
-      </c>
-      <c r="C108" s="2">
-        <v>5</v>
+        <v>424</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>210</v>
+        <v>455</v>
+      </c>
+      <c r="C109" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>333</v>
+        <v>21</v>
       </c>
       <c r="B110" t="s">
-        <v>369</v>
+        <v>41</v>
+      </c>
+      <c r="C110" t="s">
+        <v>55</v>
+      </c>
+      <c r="D110" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>430</v>
+        <v>435</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>274</v>
-      </c>
-      <c r="B112" t="s">
-        <v>368</v>
+        <v>255</v>
       </c>
       <c r="C112" t="s">
-        <v>147</v>
+        <v>257</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>68</v>
-      </c>
-      <c r="B113" t="s">
-        <v>169</v>
-      </c>
-      <c r="C113" t="s">
-        <v>46</v>
-      </c>
-      <c r="D113" t="s">
-        <v>69</v>
+        <v>412</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>441</v>
+        <v>230</v>
       </c>
       <c r="B114" t="s">
-        <v>442</v>
+        <v>367</v>
+      </c>
+      <c r="C114" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>423</v>
+        <v>210</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>99</v>
+        <v>333</v>
       </c>
       <c r="B116" t="s">
-        <v>98</v>
-      </c>
-      <c r="C116" t="s">
-        <v>59</v>
-      </c>
-      <c r="D116" t="s">
-        <v>136</v>
+        <v>369</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>331</v>
-      </c>
-      <c r="B117" t="s">
-        <v>370</v>
+        <v>430</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>313</v>
+        <v>274</v>
       </c>
       <c r="B118" t="s">
-        <v>371</v>
+        <v>368</v>
+      </c>
+      <c r="C118" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>262</v>
+        <v>68</v>
+      </c>
+      <c r="B119" t="s">
+        <v>169</v>
       </c>
       <c r="C119" t="s">
-        <v>257</v>
+        <v>46</v>
+      </c>
+      <c r="D119" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>109</v>
+        <v>441</v>
       </c>
       <c r="B120" t="s">
-        <v>171</v>
-      </c>
-      <c r="C120" t="s">
-        <v>137</v>
-      </c>
-      <c r="D120" t="s">
-        <v>138</v>
+        <v>442</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>225</v>
-      </c>
-      <c r="B121" t="s">
-        <v>372</v>
+        <v>423</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>451</v>
+        <v>99</v>
+      </c>
+      <c r="B122" t="s">
+        <v>98</v>
       </c>
       <c r="C122" t="s">
-        <v>452</v>
+        <v>59</v>
+      </c>
+      <c r="D122" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>83</v>
+        <v>331</v>
       </c>
       <c r="B123" t="s">
-        <v>261</v>
-      </c>
-      <c r="C123" t="s">
-        <v>139</v>
-      </c>
-      <c r="D123" t="s">
-        <v>140</v>
+        <v>370</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>244</v>
+        <v>313</v>
       </c>
       <c r="B124" t="s">
-        <v>265</v>
-      </c>
-      <c r="C124" t="s">
-        <v>249</v>
+        <v>371</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>460</v>
+        <v>262</v>
+      </c>
+      <c r="C125" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>246</v>
+        <v>109</v>
       </c>
       <c r="B126" t="s">
-        <v>269</v>
+        <v>171</v>
       </c>
       <c r="C126" t="s">
-        <v>249</v>
+        <v>137</v>
+      </c>
+      <c r="D126" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>465</v>
-      </c>
-      <c r="C127" t="s">
-        <v>466</v>
+        <v>225</v>
+      </c>
+      <c r="B127" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>276</v>
-      </c>
-      <c r="B128" t="s">
-        <v>373</v>
+        <v>451</v>
+      </c>
+      <c r="C128" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>226</v>
+        <v>83</v>
       </c>
       <c r="B129" t="s">
-        <v>374</v>
+        <v>261</v>
+      </c>
+      <c r="C129" t="s">
+        <v>139</v>
+      </c>
+      <c r="D129" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>405</v>
+        <v>244</v>
+      </c>
+      <c r="B130" t="s">
+        <v>265</v>
+      </c>
+      <c r="C130" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>305</v>
-      </c>
-      <c r="B131" t="s">
-        <v>306</v>
+        <v>460</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B132" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="C132" t="s">
         <v>249</v>
@@ -3043,304 +3047,298 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>302</v>
-      </c>
-      <c r="B133" t="s">
-        <v>303</v>
+        <v>465</v>
       </c>
       <c r="C133" t="s">
-        <v>213</v>
+        <v>466</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>247</v>
+        <v>276</v>
       </c>
       <c r="B134" t="s">
-        <v>266</v>
-      </c>
-      <c r="C134" t="s">
-        <v>249</v>
+        <v>373</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>248</v>
-      </c>
-      <c r="C135" t="s">
-        <v>249</v>
+        <v>226</v>
+      </c>
+      <c r="B135" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>311</v>
-      </c>
-      <c r="B136" t="s">
-        <v>375</v>
+        <v>405</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="B137" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>209</v>
+        <v>245</v>
       </c>
       <c r="B138" t="s">
-        <v>299</v>
+        <v>267</v>
+      </c>
+      <c r="C138" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="B139" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
       <c r="C139" t="s">
-        <v>292</v>
+        <v>213</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>23</v>
+        <v>247</v>
       </c>
       <c r="B140" t="s">
-        <v>77</v>
+        <v>266</v>
       </c>
       <c r="C140" t="s">
-        <v>46</v>
-      </c>
-      <c r="D140" t="s">
-        <v>72</v>
+        <v>249</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>87</v>
-      </c>
-      <c r="B141" t="s">
-        <v>172</v>
+        <v>248</v>
       </c>
       <c r="C141" t="s">
-        <v>113</v>
-      </c>
-      <c r="D141" t="s">
-        <v>130</v>
+        <v>249</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>407</v>
+        <v>311</v>
+      </c>
+      <c r="B142" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>330</v>
+        <v>297</v>
+      </c>
+      <c r="B143" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>337</v>
+        <v>209</v>
       </c>
       <c r="B144" t="s">
-        <v>376</v>
+        <v>299</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>437</v>
+        <v>294</v>
+      </c>
+      <c r="B145" t="s">
+        <v>295</v>
+      </c>
+      <c r="C145" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>212</v>
+        <v>23</v>
       </c>
       <c r="B146" t="s">
-        <v>271</v>
+        <v>77</v>
       </c>
       <c r="C146" t="s">
-        <v>213</v>
+        <v>46</v>
+      </c>
+      <c r="D146" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>24</v>
+        <v>87</v>
       </c>
       <c r="B147" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C147" t="s">
-        <v>46</v>
+        <v>113</v>
       </c>
       <c r="D147" t="s">
-        <v>73</v>
+        <v>130</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>25</v>
-      </c>
-      <c r="B148" t="s">
-        <v>174</v>
-      </c>
-      <c r="C148" t="s">
-        <v>46</v>
-      </c>
-      <c r="D148" t="s">
-        <v>62</v>
+        <v>407</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>26</v>
-      </c>
-      <c r="B149" t="s">
-        <v>175</v>
-      </c>
-      <c r="C149" t="s">
-        <v>49</v>
-      </c>
-      <c r="D149" t="s">
-        <v>141</v>
+        <v>330</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>446</v>
+        <v>337</v>
+      </c>
+      <c r="B150" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>88</v>
-      </c>
-      <c r="B151" t="s">
-        <v>89</v>
-      </c>
-      <c r="C151" t="s">
-        <v>131</v>
-      </c>
-      <c r="D151" t="s">
-        <v>130</v>
+        <v>437</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>27</v>
+        <v>212</v>
       </c>
       <c r="B152" t="s">
-        <v>100</v>
+        <v>271</v>
       </c>
       <c r="C152" t="s">
-        <v>57</v>
-      </c>
-      <c r="D152" t="s">
-        <v>142</v>
+        <v>213</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>462</v>
+        <v>24</v>
+      </c>
+      <c r="B153" t="s">
+        <v>173</v>
       </c>
       <c r="C153" t="s">
-        <v>463</v>
+        <v>46</v>
+      </c>
+      <c r="D153" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>464</v>
+        <v>25</v>
+      </c>
+      <c r="B154" t="s">
+        <v>174</v>
+      </c>
+      <c r="C154" t="s">
+        <v>46</v>
+      </c>
+      <c r="D154" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B155" t="s">
-        <v>42</v>
+        <v>175</v>
       </c>
       <c r="C155" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D155" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>316</v>
-      </c>
-      <c r="B156" t="s">
-        <v>377</v>
+        <v>446</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B157" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C157" t="s">
-        <v>49</v>
+        <v>131</v>
       </c>
       <c r="D157" t="s">
-        <v>62</v>
+        <v>130</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>272</v>
+        <v>27</v>
+      </c>
+      <c r="B158" t="s">
+        <v>100</v>
       </c>
       <c r="C158" t="s">
-        <v>139</v>
+        <v>57</v>
+      </c>
+      <c r="D158" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>432</v>
+        <v>462</v>
+      </c>
+      <c r="C159" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>90</v>
-      </c>
-      <c r="B160" t="s">
-        <v>91</v>
-      </c>
-      <c r="C160" t="s">
-        <v>46</v>
-      </c>
-      <c r="D160" t="s">
-        <v>144</v>
+        <v>464</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>431</v>
+        <v>28</v>
+      </c>
+      <c r="B161" t="s">
+        <v>42</v>
+      </c>
+      <c r="C161" t="s">
+        <v>55</v>
+      </c>
+      <c r="D161" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>277</v>
+        <v>316</v>
       </c>
       <c r="B162" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="B163" t="s">
-        <v>176</v>
+        <v>81</v>
       </c>
       <c r="C163" t="s">
-        <v>127</v>
+        <v>49</v>
       </c>
       <c r="D163" t="s">
         <v>62</v>
@@ -3348,583 +3346,642 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>82</v>
-      </c>
-      <c r="B164" t="s">
-        <v>177</v>
+        <v>272</v>
       </c>
       <c r="C164" t="s">
-        <v>145</v>
-      </c>
-      <c r="D164" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="B166" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="C166" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D166" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>232</v>
+        <v>277</v>
       </c>
       <c r="B168" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>319</v>
+        <v>29</v>
       </c>
       <c r="B169" t="s">
-        <v>380</v>
+        <v>176</v>
+      </c>
+      <c r="C169" t="s">
+        <v>127</v>
+      </c>
+      <c r="D169" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>200</v>
+        <v>82</v>
+      </c>
+      <c r="B170" t="s">
+        <v>177</v>
+      </c>
+      <c r="C170" t="s">
+        <v>145</v>
+      </c>
+      <c r="D170" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>222</v>
+        <v>440</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>282</v>
+        <v>30</v>
+      </c>
+      <c r="B172" t="s">
+        <v>78</v>
+      </c>
+      <c r="C172" t="s">
+        <v>49</v>
+      </c>
+      <c r="D172" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>223</v>
+        <v>425</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B174" t="s">
-        <v>234</v>
+        <v>379</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>192</v>
+        <v>319</v>
       </c>
       <c r="B175" t="s">
-        <v>381</v>
-      </c>
-      <c r="C175" t="s">
-        <v>193</v>
+        <v>380</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>322</v>
-      </c>
-      <c r="B176" t="s">
-        <v>323</v>
+        <v>200</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>273</v>
+        <v>222</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>321</v>
-      </c>
-      <c r="B178" t="s">
-        <v>382</v>
+        <v>282</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>409</v>
+        <v>223</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>270</v>
+        <v>233</v>
       </c>
       <c r="B180" t="s">
-        <v>383</v>
+        <v>234</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>215</v>
+        <v>192</v>
+      </c>
+      <c r="B181" t="s">
+        <v>381</v>
       </c>
       <c r="C181" t="s">
-        <v>216</v>
+        <v>193</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>214</v>
+        <v>322</v>
       </c>
       <c r="B182" t="s">
-        <v>384</v>
-      </c>
-      <c r="C182" t="s">
-        <v>213</v>
+        <v>323</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>31</v>
-      </c>
-      <c r="B183" t="s">
-        <v>43</v>
-      </c>
-      <c r="C183" s="2">
-        <v>4</v>
-      </c>
-      <c r="D183" t="s">
-        <v>62</v>
+        <v>273</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>32</v>
+        <v>321</v>
       </c>
       <c r="B184" t="s">
-        <v>44</v>
-      </c>
-      <c r="C184" t="s">
-        <v>55</v>
-      </c>
-      <c r="D184" t="s">
-        <v>137</v>
+        <v>382</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>438</v>
+        <v>409</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>406</v>
+        <v>270</v>
       </c>
       <c r="B186" t="s">
-        <v>415</v>
+        <v>383</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>403</v>
-      </c>
-      <c r="B187" t="s">
-        <v>404</v>
+        <v>215</v>
+      </c>
+      <c r="C187" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>416</v>
+        <v>214</v>
+      </c>
+      <c r="B188" t="s">
+        <v>384</v>
+      </c>
+      <c r="C188" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>256</v>
+        <v>31</v>
       </c>
       <c r="B189" t="s">
-        <v>399</v>
-      </c>
-      <c r="C189" t="s">
-        <v>257</v>
+        <v>43</v>
+      </c>
+      <c r="C189" s="2">
+        <v>4</v>
+      </c>
+      <c r="D189" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>195</v>
+        <v>32</v>
       </c>
       <c r="B190" t="s">
-        <v>398</v>
-      </c>
-      <c r="C190" s="2" t="s">
-        <v>139</v>
+        <v>44</v>
+      </c>
+      <c r="C190" t="s">
+        <v>55</v>
+      </c>
+      <c r="D190" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>324</v>
-      </c>
-      <c r="B191" t="s">
-        <v>397</v>
+        <v>438</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>414</v>
+        <v>406</v>
+      </c>
+      <c r="B192" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>286</v>
+        <v>403</v>
       </c>
       <c r="B193" t="s">
-        <v>288</v>
-      </c>
-      <c r="C193" s="2"/>
+        <v>404</v>
+      </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>105</v>
-      </c>
-      <c r="B194" t="s">
-        <v>178</v>
-      </c>
-      <c r="C194" t="s">
-        <v>147</v>
-      </c>
-      <c r="D194" t="s">
-        <v>62</v>
+        <v>416</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>106</v>
+        <v>256</v>
       </c>
       <c r="B195" t="s">
-        <v>179</v>
+        <v>399</v>
       </c>
       <c r="C195" t="s">
-        <v>148</v>
-      </c>
-      <c r="D195" t="s">
-        <v>149</v>
+        <v>257</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>107</v>
+        <v>195</v>
       </c>
       <c r="B196" t="s">
-        <v>180</v>
-      </c>
-      <c r="C196" t="s">
-        <v>148</v>
-      </c>
-      <c r="D196" t="s">
-        <v>150</v>
+        <v>398</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="B197" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>235</v>
-      </c>
-      <c r="B198" t="s">
-        <v>395</v>
+        <v>414</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>181</v>
+        <v>286</v>
       </c>
       <c r="B199" t="s">
-        <v>182</v>
-      </c>
-      <c r="C199" t="s">
-        <v>151</v>
-      </c>
-      <c r="D199" t="s">
-        <v>152</v>
-      </c>
+        <v>288</v>
+      </c>
+      <c r="C199" s="2"/>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>328</v>
+        <v>105</v>
       </c>
       <c r="B200" t="s">
-        <v>393</v>
+        <v>178</v>
+      </c>
+      <c r="C200" t="s">
+        <v>147</v>
+      </c>
+      <c r="D200" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
       <c r="B201" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C201" t="s">
-        <v>49</v>
+        <v>148</v>
       </c>
       <c r="D201" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>433</v>
+        <v>107</v>
+      </c>
+      <c r="B202" t="s">
+        <v>180</v>
+      </c>
+      <c r="C202" t="s">
+        <v>148</v>
+      </c>
+      <c r="D202" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>194</v>
+        <v>318</v>
       </c>
       <c r="B203" t="s">
-        <v>394</v>
-      </c>
-      <c r="C203" t="s">
-        <v>193</v>
+        <v>396</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>411</v>
+        <v>235</v>
+      </c>
+      <c r="B204" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>427</v>
+        <v>181</v>
+      </c>
+      <c r="B205" t="s">
+        <v>182</v>
+      </c>
+      <c r="C205" t="s">
+        <v>151</v>
+      </c>
+      <c r="D205" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>189</v>
+        <v>328</v>
       </c>
       <c r="B206" t="s">
-        <v>190</v>
-      </c>
-      <c r="C206" t="s">
-        <v>147</v>
+        <v>393</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>196</v>
-      </c>
-      <c r="B207" t="s">
-        <v>390</v>
+        <v>474</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>224</v>
+        <v>33</v>
       </c>
       <c r="B208" t="s">
-        <v>389</v>
+        <v>183</v>
+      </c>
+      <c r="C208" t="s">
+        <v>49</v>
+      </c>
+      <c r="D208" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>34</v>
-      </c>
-      <c r="B209" t="s">
-        <v>79</v>
-      </c>
-      <c r="C209" s="2">
-        <v>1</v>
-      </c>
-      <c r="D209" t="s">
-        <v>136</v>
+        <v>433</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>35</v>
+        <v>194</v>
       </c>
       <c r="B210" t="s">
-        <v>184</v>
-      </c>
-      <c r="C210" s="2">
-        <v>4</v>
-      </c>
-      <c r="D210" t="s">
-        <v>154</v>
+        <v>394</v>
+      </c>
+      <c r="C210" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>325</v>
-      </c>
-      <c r="B211" t="s">
-        <v>326</v>
-      </c>
-      <c r="C211" s="2"/>
+        <v>411</v>
+      </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>22</v>
-      </c>
-      <c r="B212" t="s">
-        <v>170</v>
-      </c>
-      <c r="C212" t="s">
-        <v>70</v>
-      </c>
-      <c r="D212" t="s">
-        <v>71</v>
+        <v>427</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>413</v>
+        <v>189</v>
+      </c>
+      <c r="B213" t="s">
+        <v>190</v>
+      </c>
+      <c r="C213" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="B214" t="s">
-        <v>388</v>
-      </c>
-      <c r="C214" s="2" t="s">
-        <v>207</v>
+        <v>390</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>36</v>
+        <v>224</v>
       </c>
       <c r="B215" t="s">
-        <v>45</v>
-      </c>
-      <c r="C215" s="2">
-        <v>4</v>
-      </c>
-      <c r="D215" t="s">
-        <v>155</v>
+        <v>389</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
       <c r="B216" t="s">
-        <v>185</v>
-      </c>
-      <c r="C216" t="s">
-        <v>46</v>
+        <v>79</v>
+      </c>
+      <c r="C216" s="2">
+        <v>1</v>
       </c>
       <c r="D216" t="s">
-        <v>62</v>
+        <v>136</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>240</v>
+        <v>35</v>
       </c>
       <c r="B217" t="s">
-        <v>241</v>
+        <v>184</v>
+      </c>
+      <c r="C217" s="2">
+        <v>4</v>
+      </c>
+      <c r="D217" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>112</v>
+        <v>325</v>
       </c>
       <c r="B218" t="s">
-        <v>186</v>
-      </c>
-      <c r="C218" t="s">
-        <v>59</v>
-      </c>
-      <c r="D218" t="s">
-        <v>156</v>
-      </c>
+        <v>326</v>
+      </c>
+      <c r="C218" s="2"/>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>287</v>
+        <v>22</v>
       </c>
       <c r="B219" t="s">
-        <v>387</v>
+        <v>170</v>
+      </c>
+      <c r="C219" t="s">
+        <v>70</v>
+      </c>
+      <c r="D219" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>37</v>
-      </c>
-      <c r="B220" t="s">
-        <v>187</v>
-      </c>
-      <c r="C220" t="s">
-        <v>120</v>
-      </c>
-      <c r="D220" t="s">
-        <v>62</v>
+        <v>413</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>391</v>
+        <v>208</v>
       </c>
       <c r="B221" t="s">
-        <v>392</v>
+        <v>388</v>
+      </c>
+      <c r="C221" s="2" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B222" t="s">
-        <v>188</v>
-      </c>
-      <c r="C222" t="s">
-        <v>64</v>
+        <v>45</v>
+      </c>
+      <c r="C222" s="2">
+        <v>4</v>
       </c>
       <c r="D222" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>428</v>
+        <v>95</v>
       </c>
       <c r="B223" t="s">
-        <v>429</v>
+        <v>185</v>
+      </c>
+      <c r="C223" t="s">
+        <v>46</v>
+      </c>
+      <c r="D223" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
+        <v>240</v>
+      </c>
+      <c r="B224" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A225" t="s">
+        <v>112</v>
+      </c>
+      <c r="B225" t="s">
+        <v>186</v>
+      </c>
+      <c r="C225" t="s">
+        <v>59</v>
+      </c>
+      <c r="D225" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A226" t="s">
+        <v>287</v>
+      </c>
+      <c r="B226" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A227" t="s">
+        <v>37</v>
+      </c>
+      <c r="B227" t="s">
+        <v>187</v>
+      </c>
+      <c r="C227" t="s">
+        <v>120</v>
+      </c>
+      <c r="D227" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A228" t="s">
+        <v>391</v>
+      </c>
+      <c r="B228" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A229" t="s">
+        <v>38</v>
+      </c>
+      <c r="B229" t="s">
+        <v>188</v>
+      </c>
+      <c r="C229" t="s">
+        <v>64</v>
+      </c>
+      <c r="D229" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A230" t="s">
+        <v>428</v>
+      </c>
+      <c r="B230" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A231" t="s">
         <v>317</v>
       </c>
-      <c r="B224" t="s">
+      <c r="B231" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A225" t="s">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A232" t="s">
         <v>275</v>
       </c>
-      <c r="B225" t="s">
+      <c r="B232" t="s">
         <v>385</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D225">
-    <sortCondition ref="A71"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D232">
+    <sortCondition ref="A76"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>